<commit_message>
Add: Code Responses for Guided APR
</commit_message>
<xml_diff>
--- a/Analysis/QuixBugs_GPT_APR/APR_one_shot_ChatGPT_3.5_turbo_Java.xlsx
+++ b/Analysis/QuixBugs_GPT_APR/APR_one_shot_ChatGPT_3.5_turbo_Java.xlsx
@@ -1,17 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Investigation Proper\Bug-Busters\Analysis\QuixBugs_GPT_APR\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21030CB-0324-47AC-8B3B-A9B9ED6DD1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="APR_one_shot_ChatGPT_3.5_turbo_" sheetId="1" r:id="rId4"/>
+    <sheet name="APR_one_shot_ChatGPT_3.5_turbo_" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="301">
   <si>
     <t>File Name</t>
   </si>
@@ -3780,59 +3802,1548 @@
     return lines;
 }</t>
   </si>
+  <si>
+    <t>Correct Code</t>
+  </si>
+  <si>
+    <t>Expected Line with Bug</t>
+  </si>
+  <si>
+    <t>Correct Response</t>
+  </si>
+  <si>
+    <t>Test Cases (For responses that are not identical to the correct code)</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+_x000D_
+_x000D_
+public class BITCOUNT {_x000D_
+    public static int bitcount(int n) {_x000D_
+    int count = 0;_x000D_
+    while (n != 0) {_x000D_
+        n = (n &amp; (n - 1));_x000D_
+        count++;_x000D_
+    }_x000D_
+    return count;_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>n = (n ^ (n - 1));</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+import java.util.ArrayDeque;_x000D_
+_x000D_
+import java_programs.Node;_x000D_
+_x000D_
+_x000D_
+public class BREADTH_FIRST_SEARCH {_x000D_
+_x000D_
+    public static Set&lt;Node&gt; nodesvisited = new HashSet&lt;&gt;();_x000D_
+_x000D_
+    public static boolean breadth_first_search(Node startnode, Node goalnode) {_x000D_
+        Deque&lt;Node&gt; queue = new ArrayDeque&lt;&gt;();_x000D_
+        queue.addLast(startnode);_x000D_
+_x000D_
+        nodesvisited.add(startnode);_x000D_
+_x000D_
+        while (!queue.isEmpty()) {_x000D_
+            Node node = queue.removeFirst();_x000D_
+_x000D_
+            if (node == goalnode) {_x000D_
+                return true;_x000D_
+            } else {_x000D_
+                for (Node successor_node : node.getSuccessors()) {_x000D_
+                    if (!nodesvisited.contains(successor_node)) {_x000D_
+                        queue.addFirst(successor_node);_x000D_
+                        nodesvisited.add(successor_node);_x000D_
+                    }_x000D_
+                }_x000D_
+            }_x000D_
+        }_x000D_
+         return false;_x000D_
+    }_x000D_
+_x000D_
+}</t>
+  </si>
+  <si>
+    <t>while (true) {</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class BUCKETSORT {_x000D_
+    public static ArrayList&lt;Integer&gt; bucketsort(ArrayList&lt;Integer&gt; arr, int k) {_x000D_
+        ArrayList&lt;Integer&gt; counts = new ArrayList&lt;Integer&gt;(Collections.nCopies(k,0));_x000D_
+        for (Integer x : arr) {_x000D_
+            counts.set(x,counts.get(x)+1);_x000D_
+        }_x000D_
+_x000D_
+        ArrayList&lt;Integer&gt; sorted_arr = new ArrayList&lt;Integer&gt;(100);_x000D_
+        int i = 0;_x000D_
+        for (Integer count : counts) {_x000D_
+            sorted_arr.addAll(Collections.nCopies(count, i));_x000D_
+            i++;_x000D_
+        }_x000D_
+_x000D_
+        return sorted_arr;_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>for (Integer count : arr) {</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+import java_programs.Node;
+public class DEPTH_FIRST_SEARCH {
+    public static boolean depth_first_search(Node startnode, Node goalnode) {
+        Set&lt;Node&gt; nodesvisited = new HashSet&lt;&gt;();
+        class Search {
+            boolean search(Node node) {
+                if (nodesvisited.contains(node)) {
+                    return false;
+                } else if (node == goalnode) {
+                    return true;
+                } else {
+                        nodesvisited.add(node);
+                    for (Node successornodes : node.getSuccessors()) {
+                        if (search(successornodes)) { return true; }
+                    }
+                }
+                return false;
+            }
+        };
+        Search s = new Search();
+        return s.search(startnode);
+    }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Omission - Within the else statement.
+} else {
+                        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nodesvisited.add(node);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                    for (Node successornodes : node.getSuccessors()) {
+                        if (search(successornodes)) { return true; }
+                    }</t>
+    </r>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+import java_programs.Node;_x000D_
+_x000D_
+public class DETECT_CYCLE {_x000D_
+    public static boolean detect_cycle(Node node) {_x000D_
+        Node hare = node;_x000D_
+        Node tortoise = node;_x000D_
+_x000D_
+        while (true) {_x000D_
+            if (null==hare ||hare.getSuccessor() == null)_x000D_
+                return false;_x000D_
+_x000D_
+            tortoise = tortoise.getSuccessor();_x000D_
+            hare = hare.getSuccessor().getSuccessor();_x000D_
+_x000D_
+            if (hare == tortoise)_x000D_
+                return true;_x000D_
+        }_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>if (hare.getSuccessor() == null)</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class FIND_FIRST_IN_SORTED {_x000D_
+_x000D_
+    public static int find_first_in_sorted(int[] arr, int x) {_x000D_
+        int lo = 0;_x000D_
+        int hi = arr.length;_x000D_
+_x000D_
+        while (lo &lt; hi) {_x000D_
+            int mid = (lo + hi) / 2; // check if this is floor division_x000D_
+_x000D_
+            if (x == arr[mid] &amp;&amp; (mid == 0 || x != arr[mid-1])) {_x000D_
+                return mid;_x000D_
+            } else if (x &lt;= arr[mid]) {_x000D_
+                hi = mid;_x000D_
+            } else {_x000D_
+                lo = mid + 1;_x000D_
+            }_x000D_
+        }_x000D_
+_x000D_
+        return -1;_x000D_
+    }_x000D_
+_x000D_
+}</t>
+  </si>
+  <si>
+    <t>while (lo &lt;= hi) {</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+_x000D_
+_x000D_
+public class FIND_IN_SORTED {_x000D_
+    public static int binsearch(int[] arr, int x, int start, int end) {_x000D_
+        if (start == end) {_x000D_
+            return -1;_x000D_
+        }_x000D_
+        int mid = start + (end - start) / 2; // check this is floor division_x000D_
+        if (x &lt; arr[mid]) {_x000D_
+            return binsearch(arr, x, start, mid);_x000D_
+        } else if (x &gt; arr[mid]) {_x000D_
+            return binsearch(arr, x, mid+1, end);_x000D_
+        } else {_x000D_
+            return mid;_x000D_
+        }_x000D_
+    }_x000D_
+_x000D_
+    public static int find_in_sorted(int[] arr, int x) {_x000D_
+        return binsearch(arr, x, 0, arr.length);_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>return binsearch(arr, x, mid, end);</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class FLATTEN {_x000D_
+    public static Object flatten(Object arr) {_x000D_
+        if (arr instanceof ArrayList) {_x000D_
+            ArrayList narr = (ArrayList) arr;_x000D_
+            ArrayList result = new ArrayList(50);_x000D_
+            for (Object x : narr) {_x000D_
+                if (x instanceof ArrayList) {_x000D_
+                    result.addAll((ArrayList) flatten(x));_x000D_
+                } else {_x000D_
+                    result.add((x));_x000D_
+                }_x000D_
+            }_x000D_
+            return result;_x000D_
+        } else {_x000D_
+            return arr;_x000D_
+        }_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>Two errors: 
+result.add(flatten(x)); and
+return flatten(arr);</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class GCD {_x000D_
+_x000D_
+    public static int gcd(int a, int b) {_x000D_
+        if (b == 0) {_x000D_
+            return a;_x000D_
+        } else {_x000D_
+            return gcd(b, a%b);_x000D_
+        }_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>return gcd(a % b, b);</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class GET_FACTORS {_x000D_
+    public static ArrayList&lt;Integer&gt; get_factors(int n) {_x000D_
+        if (n == 1) {_x000D_
+            return new ArrayList&lt;Integer&gt;();_x000D_
+        }_x000D_
+        int max = (int)(Math.sqrt(n) + 1.0);_x000D_
+        for (int i=2; i &lt; max; i++) {_x000D_
+            if (n % i == 0) {_x000D_
+                ArrayList&lt;Integer&gt; prepend = new ArrayList&lt;Integer&gt;(0);_x000D_
+                prepend.add(i);_x000D_
+                prepend.addAll(get_factors(n / i));_x000D_
+                return prepend;_x000D_
+            }_x000D_
+        }_x000D_
+_x000D_
+        return new ArrayList&lt;Integer&gt;(Arrays.asList(n));_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>return new ArrayList&lt;Integer&gt;();</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class HANOI {_x000D_
+    public static List&lt;Pair&lt;Integer,Integer&gt;&gt; hanoi(int height, int start, int end) {_x000D_
+        ArrayList&lt;Pair&lt;Integer,Integer&gt;&gt; steps = new ArrayList&lt;Pair&lt;Integer,Integer&gt;&gt;();_x000D_
+_x000D_
+        if (height &gt; 0) {_x000D_
+            PriorityQueue&lt;Integer&gt; crap_set = new PriorityQueue&lt;Integer&gt;();_x000D_
+            crap_set.add(1);_x000D_
+            crap_set.add(2);_x000D_
+            crap_set.add(3);_x000D_
+            crap_set.remove(start);_x000D_
+            crap_set.remove(end);_x000D_
+            int helper = crap_set.poll();_x000D_
+            steps.addAll(hanoi(height-1, start, helper));_x000D_
+            steps.add(new Pair&lt;Integer,Integer&gt;(start, end));_x000D_
+            steps.addAll(hanoi(height-1, helper, end));_x000D_
+        }_x000D_
+_x000D_
+        return steps;_x000D_
+    }_x000D_
+_x000D_
+_x000D_
+    public static class Pair&lt;F, S&gt; {_x000D_
+        private F first; //first member of pair_x000D_
+        private S second; //second member of pair_x000D_
+_x000D_
+        public Pair(F first, S second) {_x000D_
+            this.first = first;_x000D_
+            this.second = second;_x000D_
+        }_x000D_
+_x000D_
+        public void setFirst(F first) {_x000D_
+            this.first = first;_x000D_
+        }_x000D_
+_x000D_
+        public void setSecond(S second) {_x000D_
+            this.second = second;_x000D_
+        }_x000D_
+_x000D_
+        public F getFirst() {_x000D_
+            return first;_x000D_
+        }_x000D_
+_x000D_
+        public S getSecond() {_x000D_
+            return second;_x000D_
+        }_x000D_
+_x000D_
+        @Override_x000D_
+        public String toString() {_x000D_
+            return "(" + String.valueOf(first) + ", " + String.valueOf(second) + ")";_x000D_
+        }_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>steps.add(new Pair&lt;Integer,Integer&gt;(start, helper));</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class IS_VALID_PARENTHESIZATION {_x000D_
+    public static Boolean is_valid_parenthesization(String parens) {_x000D_
+        int depth = 0;_x000D_
+        for (int i = 0; i &lt; parens.length(); i++) {_x000D_
+            Character paren = parens.charAt(i);_x000D_
+            if (paren.equals('(')) {_x000D_
+                depth++;_x000D_
+            } else {_x000D_
+                depth--;_x000D_
+                if (depth &lt; 0) { return false; }_x000D_
+            }_x000D_
+        }_x000D_
+        return depth==0;_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>return true;</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class KHEAPSORT {_x000D_
+_x000D_
+    public static ArrayList&lt;Integer&gt; kheapsort(ArrayList&lt;Integer&gt; arr, int k) {_x000D_
+        PriorityQueue&lt;Integer&gt; heap = new PriorityQueue&lt;Integer&gt;();_x000D_
+        for (Integer v : arr.subList(0,k)) {_x000D_
+            heap.add(v);_x000D_
+        }_x000D_
+_x000D_
+        ArrayList&lt;Integer&gt; output = new ArrayList&lt;Integer&gt;();_x000D_
+        for (Integer x : arr.subList(k, arr.size())) {_x000D_
+            heap.add(x);_x000D_
+            Integer popped = heap.poll();_x000D_
+            output.add(popped);_x000D_
+        }_x000D_
+_x000D_
+        while (!heap.isEmpty()) {_x000D_
+            output.add(heap.poll());_x000D_
+        }_x000D_
+_x000D_
+        return output;_x000D_
+_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>for (Integer x : arr) {</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+import java.lang.*;_x000D_
+_x000D_
+_x000D_
+public class KNAPSACK {_x000D_
+    public static int knapsack(int capacity, int [][] items) {_x000D_
+        int weight = 0, value = 0;_x000D_
+        int n = items.length;_x000D_
+        int memo[][] = new int[n + 1][capacity + 1];_x000D_
+_x000D_
+        for (int i = 0; i &lt;= n ; i++)_x000D_
+        {_x000D_
+            if (i - 1 &gt;= 0) {_x000D_
+                weight = items[i - 1][0];_x000D_
+                value = items[i - 1][1];_x000D_
+            }_x000D_
+            for (int j = 0; j &lt;= capacity; j++)_x000D_
+            {_x000D_
+                if (i == 0 || j == 0) {_x000D_
+                    memo[i][j] = 0;_x000D_
+                }_x000D_
+                else if (weight &lt;= j) {_x000D_
+                    memo[i][j] = Math.max(memo[i - 1][j], value + memo[i - 1][j - weight]);_x000D_
+                }_x000D_
+                else {_x000D_
+                    memo[i][j] = memo [i-1][j];_x000D_
+                }_x000D_
+_x000D_
+            }_x000D_
+        }_x000D_
+        return memo[n][capacity];_x000D_
+    }_x000D_
+_x000D_
+}</t>
+  </si>
+  <si>
+    <t>else if (weight &lt; j) {</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class KTH {_x000D_
+    public static Integer kth(ArrayList&lt;Integer&gt; arr, int k) {_x000D_
+        int pivot = arr.get(0);_x000D_
+        ArrayList&lt;Integer&gt; below, above;_x000D_
+        below = new ArrayList&lt;Integer&gt;(arr.size());_x000D_
+        above = new ArrayList&lt;Integer&gt;(arr.size());_x000D_
+        for (Integer x : arr) {_x000D_
+            if (x &lt; pivot) {_x000D_
+                below.add(x);_x000D_
+            } else if (x &gt; pivot) {_x000D_
+                above.add(x);_x000D_
+            }_x000D_
+        }_x000D_
+_x000D_
+        int num_less = below.size();_x000D_
+        int num_lessoreq = arr.size() - above.size();_x000D_
+        if (k &lt; num_less) {_x000D_
+            return kth(below, k);_x000D_
+        } else if (k &gt;= num_lessoreq) {_x000D_
+            return kth(above, k-num_lessoreq);_x000D_
+        } else {_x000D_
+            return pivot;_x000D_
+        }_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>return kth(above, k);</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+public class LCS_LENGTH {
+    public static Integer lcs_length(String s, String t) {
+        Map&lt;Integer, Map&lt;Integer,Integer&gt;&gt; dp = new HashMap&lt;Integer,Map&lt;Integer,Integer&gt;&gt;();
+        for (int i=0; i &lt; s.length(); i++) {
+            Map&lt;Integer,Integer&gt; initialize = new HashMap&lt;Integer,Integer&gt;();
+            dp.put(i, initialize);
+            for (int j=0; j &lt; t.length(); j++) {
+                Map&lt;Integer,Integer&gt; internal_map = dp.get(i);
+                internal_map.put(j,0);
+                dp.put(i, internal_map);
+            }
+        }
+        for (int i=0; i &lt; s.length(); i++) {
+            for (int j=0; j &lt; t.length(); j++) {
+                if (s.charAt(i) == t.charAt(j)) {
+                    if (dp.containsKey(i-1)&amp;&amp;dp.get(i-1).containsKey(j-1)) {
+                        Map&lt;Integer, Integer&gt; internal_map = dp.get(i);
+                        int insert_value = dp.get(i-1).get(j-1) + 1;
+                        internal_map.put(j, insert_value);
+                        dp.put(i,internal_map);
+                    } else {
+                        Map&lt;Integer, Integer&gt; internal_map = dp.get(i);
+                        internal_map.put(j,1);
+                        dp.put(i,internal_map);
+                    }
+                }
+            }
+        }
+        if (!dp.isEmpty()) {
+            List&lt;Integer&gt; ret_list = new ArrayList&lt;Integer&gt;();
+            for (int i=0; i&lt;s.length(); i++) {
+                ret_list.add(!dp.get(i).isEmpty() ? Collections.max(dp.get(i).values()) : 0);
+            }
+            return Collections.max(ret_list);
+        } else {
+            return 0;
+        }
+    }
+}</t>
+  </si>
+  <si>
+    <t>if (dp.containsKey(i-1)) {</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+public class LEVENSHTEIN {_x000D_
+    public static int levenshtein(String source, String target) {_x000D_
+        if (source.isEmpty() || target.isEmpty()) {_x000D_
+            return source.isEmpty() ? target.length() : source.length();_x000D_
+        } else if (source.charAt(0) == target.charAt(0)) {_x000D_
+            return levenshtein(source.substring(1), target.substring(1));_x000D_
+        } else {_x000D_
+            return 1 + Math.min(Math.min(_x000D_
+                    levenshtein(source,              target.substring(1)),_x000D_
+                    levenshtein(source.substring(1), target.substring(1))),_x000D_
+                    levenshtein(source.substring(1), target)_x000D_
+        );_x000D_
+        }_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>return 1 + levenshtein(source.substring(1), target.substring(1));</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+public class LIS {_x000D_
+    public static int lis(int[] arr) {_x000D_
+        Map&lt;Integer,Integer&gt; ends = new HashMap&lt;Integer, Integer&gt;(100);_x000D_
+        int longest = 0;_x000D_
+_x000D_
+        int i = 0;_x000D_
+        for (int val : arr) {_x000D_
+_x000D_
+            ArrayList&lt;Integer&gt; prefix_lengths = new ArrayList&lt;Integer&gt;(100);_x000D_
+            for (int j=1; j &lt; longest+1; j++) {_x000D_
+                if (arr[ends.get(j)] &lt; val) {_x000D_
+                    prefix_lengths.add(j);_x000D_
+                }_x000D_
+            }_x000D_
+_x000D_
+            int length = !prefix_lengths.isEmpty() ? Collections.max(prefix_lengths) : 0;_x000D_
+_x000D_
+            if (length == longest || val &lt; arr[ends.get(length+1)]) {_x000D_
+                ends.put(length+1, i);_x000D_
+                longest = Math.max(longest,length + 1);_x000D_
+            }_x000D_
+_x000D_
+            i++;_x000D_
+        }_x000D_
+        return longest;_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>longest = length + 1;</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class LONGEST_COMMON_SUBSEQUENCE {_x000D_
+    public static String longest_common_subsequence(String a, String b) {_x000D_
+        if (a.isEmpty() || b.isEmpty()) {_x000D_
+            return "";_x000D_
+        } else if (a.charAt(0) == b.charAt(0)) {_x000D_
+            return a.charAt(0) + longest_common_subsequence(a.substring(1), b.substring(1));_x000D_
+        } else {_x000D_
+            String fst = longest_common_subsequence(a, b.substring(1));_x000D_
+            String snd = longest_common_subsequence(a.substring(1), b);_x000D_
+            return fst.length() &gt;= snd.length() ? fst : snd;_x000D_
+        }_x000D_
+_x000D_
+    }_x000D_
+_x000D_
+}</t>
+  </si>
+  <si>
+    <t>return a.charAt(0) + longest_common_subsequence(a.substring(1), b);</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class MAX_SUBLIST_SUM {_x000D_
+    public static int max_sublist_sum(int[] arr) {_x000D_
+        int max_ending_here = 0;_x000D_
+        int max_so_far = 0;_x000D_
+_x000D_
+        for (int x : arr) {_x000D_
+            max_ending_here = Math.max(0,max_ending_here + x);_x000D_
+            max_so_far = Math.max(max_so_far, max_ending_here);_x000D_
+        }_x000D_
+_x000D_
+        return max_so_far;_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>max_ending_here = max_ending_here + x;</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+public class MERGESORT {
+    public static ArrayList&lt;Integer&gt; merge(ArrayList&lt;Integer&gt; left, ArrayList&lt;Integer&gt; right) {
+        ArrayList&lt;Integer&gt; result = new ArrayList&lt;Integer&gt;(100);
+        int i = 0;
+        int j = 0;
+        while (i &lt; left.size() &amp;&amp; j &lt; right.size()) {
+            if (left.get(i) &lt;= right.get(j)) {
+                result.add(left.get(i));
+                i++;
+            } else {
+                result.add(right.get(j));
+                j++;
+            }
+        }
+        result.addAll(left.subList(i,left.size()).isEmpty() ? right.subList(j, right.size()) : left.subList(i, left.size()));
+        return result;
+    }
+    public static ArrayList&lt;Integer&gt; mergesort(ArrayList&lt;Integer&gt; arr) {
+        if (arr.size() &lt;= 1) { // &lt;= 1 in correct version
+            return arr;
+        } else {
+            int middle = arr.size() / 2;
+            ArrayList&lt;Integer&gt; left = new ArrayList&lt;Integer&gt;(100);
+            left.addAll(arr.subList(0,middle));
+            left = mergesort(left);
+            ArrayList&lt;Integer&gt; right = new ArrayList&lt;Integer&gt;(100);
+            right.addAll(arr.subList(middle, arr.size()));
+            right = mergesort(right);
+            return merge(left, right);
+        }
+    }
+}</t>
+  </si>
+  <si>
+    <t>if (arr.size() == 0) { // &lt;= 1 in correct version</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+import java_programs.Node;
+import java_programs.WeightedEdge;
+public class MINIMUM_SPANNING_TREE {
+    public static Set&lt;WeightedEdge&gt; minimum_spanning_tree(List&lt;WeightedEdge&gt; weightedEdges) {
+        Map&lt;Node,Set&lt;Node&gt;&gt; groupByNode = new HashMap&lt;&gt;();
+        Set&lt;WeightedEdge&gt; minSpanningTree = new HashSet&lt;&gt;();
+        Collections.sort(weightedEdges);
+        for (WeightedEdge edge : weightedEdges) {
+            Node vertex_u = edge.node1;
+            Node vertex_v = edge.node2;
+            if (!groupByNode.containsKey(vertex_u)){
+                groupByNode.put(vertex_u, new HashSet&lt;&gt;(Arrays.asList(vertex_u)));
+            }
+            if (!groupByNode.containsKey(vertex_v)){
+                groupByNode.put(vertex_v, new HashSet&lt;&gt;(Arrays.asList(vertex_v)));
+            }
+            if (groupByNode.get(vertex_u) != groupByNode.get(vertex_v)) {
+                minSpanningTree.add(edge);
+                groupByNode = update(groupByNode, vertex_u, vertex_v);
+                for (Node node : groupByNode.get(vertex_v)) {
+                    groupByNode.put(node,  groupByNode.get(vertex_u));
+                }
+            }
+        }
+        return minSpanningTree;
+    }
+    public static Map&lt;Node,Set&lt;Node&gt;&gt; update(Map&lt;Node,Set&lt;Node&gt;&gt; groupByNode, Node vertex_u, Node vertex_v) {
+        Set&lt;Node&gt; vertex_u_span = groupByNode.get(vertex_u);
+        vertex_u_span.addAll(groupByNode.get(vertex_v));
+        return groupByNode;
+    }
+}</t>
+  </si>
+  <si>
+    <t>groupByNode = update(groupByNode, node, vertex_u);</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+import java.lang.Math.*;
+public class NEXT_PALINDROME {
+    public static String next_palindrome(int[] digit_list) {
+        int high_mid = Math.floorDiv(digit_list.length, 2);
+        int low_mid = Math.floorDiv(digit_list.length - 1, 2);
+        while (high_mid &lt; digit_list.length &amp;&amp; low_mid &gt;= 0) {
+            if (digit_list[high_mid] == 9) {
+                digit_list[high_mid] = 0;
+                digit_list[low_mid] = 0;
+                high_mid += 1;
+                low_mid -= 1;
+            } else {
+                digit_list[high_mid] += 1;
+                if (low_mid != high_mid) {
+                    digit_list[low_mid] += 1;
+                }
+                return Arrays.toString(digit_list);
+            }
+        }
+        ArrayList&lt;Integer&gt; otherwise = new ArrayList&lt;Integer&gt;();
+        otherwise.add(1);
+        otherwise.addAll(Collections.nCopies(digit_list.length-1, 0));
+        otherwise.add(1);
+        return String.valueOf(otherwise);
+    }
+}</t>
+  </si>
+  <si>
+    <t>otherwise.addAll(Collections.nCopies(digit_list.length, 0));</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class NEXT_PERMUTATION {_x000D_
+    public static ArrayList&lt;Integer&gt; next_permutation(ArrayList&lt;Integer&gt; perm) {_x000D_
+        for (int i=perm.size()-2; i!=-1; i--) {_x000D_
+            if (perm.get(i) &lt; perm.get(i+1)) {_x000D_
+                for (int j=perm.size()-1; j!=i; j--) {_x000D_
+                    if (perm.get(j) &gt; perm.get(i)) {_x000D_
+                        ArrayList&lt;Integer&gt; next_perm = perm;_x000D_
+                        int temp_j = perm.get(j);_x000D_
+                        int temp_i = perm.get(i);_x000D_
+                        next_perm.set(i,temp_j);_x000D_
+                        next_perm.set(j,temp_i);_x000D_
+_x000D_
+                        ArrayList&lt;Integer&gt; reversed = new ArrayList&lt;Integer&gt;(100);_x000D_
+                        for (int k=next_perm.size()-1; k!=i; k--) {_x000D_
+                            reversed.add(next_perm.get(k));_x000D_
+                        }_x000D_
+_x000D_
+                        int q = i + 1;_x000D_
+                        for (Integer replace : reversed) {_x000D_
+                            next_perm.set(q, replace);_x000D_
+                            q++;_x000D_
+                        }_x000D_
+_x000D_
+                        return next_perm;_x000D_
+                    }_x000D_
+                }_x000D_
+            }_x000D_
+        }_x000D_
+_x000D_
+        return new ArrayList&lt;Integer&gt;();_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>if (perm.get(j) &lt; perm.get(i)) {</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class PASCAL {_x000D_
+    public static ArrayList&lt;ArrayList&lt;Integer&gt;&gt; pascal(int n) {_x000D_
+        ArrayList&lt;ArrayList&lt;Integer&gt;&gt; rows = new ArrayList&lt;ArrayList&lt;Integer&gt;&gt;();_x000D_
+        ArrayList&lt;Integer&gt; init = new ArrayList&lt;Integer&gt;();_x000D_
+        init.add(1);_x000D_
+        rows.add(init);_x000D_
+_x000D_
+        for (int r=1; r&lt;n; r++) {_x000D_
+            ArrayList&lt;Integer&gt; row = new ArrayList&lt;Integer&gt;();_x000D_
+            for (int c=0; c&lt;r+1; c++) {_x000D_
+                int upleft, upright;_x000D_
+                if (c &gt; 0) {_x000D_
+                    upleft = rows.get(r-1).get(c-1);_x000D_
+                } else {_x000D_
+                    upleft = 0;_x000D_
+                }_x000D_
+                if (c &lt; r) {_x000D_
+                    upright = rows.get(r-1).get(c);_x000D_
+                } else {_x000D_
+                    upright = 0;_x000D_
+                }_x000D_
+                row.add(upleft+upright);_x000D_
+            }_x000D_
+            rows.add(row);_x000D_
+        }_x000D_
+_x000D_
+        return rows;_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>for (int c=0; c&lt;r; c++) {</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+public class POSSIBLE_CHANGE {_x000D_
+    public static int possible_change(int[] coins, int total) {_x000D_
+        if (total == 0) {_x000D_
+            return 1;_x000D_
+        }_x000D_
+        if (total &lt; 0 ||coins.length==0) {_x000D_
+            return 0;_x000D_
+        }_x000D_
+_x000D_
+        int first = coins[0];_x000D_
+        int[] rest = Arrays.copyOfRange(coins, 1, coins.length);_x000D_
+        return possible_change(coins, total-first) + possible_change(rest, total);_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>if (total &lt; 0) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">package correct_java_programs;
+import java.util.*;
+public class POWERSET {
+    public static ArrayList&lt;ArrayList&gt; powerset(ArrayList arr) {
+        if (!arr.isEmpty()) {
+            Object first = arr.get(0);
+            arr.remove(0);
+            ArrayList rest = arr;
+            ArrayList&lt;ArrayList&gt; rest_subsets = powerset(rest);
+            ArrayList&lt;ArrayList&gt; output = new ArrayList&lt;ArrayList&gt;(100);
+            ArrayList to_add = new ArrayList(100);
+            for (ArrayList subset : rest_subsets) {
+                ArrayList r = new ArrayList();
+                r.add(first);
+                r.addAll(subset);
+                to_add.add(r);
+            }
+            output.addAll(to_add);
+            rest_subsets.addAll(output);
+            return rest_subsets;
+        } else {
+            ArrayList empty_set = new ArrayList&lt;ArrayList&gt;();
+            empty_set.add(new ArrayList());
+            return empty_set;
+        }
+    }
+}
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Addition: 
+to_add.add(first);
+Omission:
+ for (ArrayList subset : rest_subsets) {
+                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ArrayList r = new ArrayList();
+                r.add(first);
+                r.addAll(subset);
+                to_add.add(r);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">            }</t>
+    </r>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class QUICKSORT {_x000D_
+    public static ArrayList&lt;Integer&gt; quicksort(ArrayList&lt;Integer&gt; arr) {_x000D_
+        if (arr.isEmpty()) {_x000D_
+            return new ArrayList&lt;Integer&gt;();_x000D_
+        }_x000D_
+_x000D_
+        Integer pivot = arr.get(0);_x000D_
+        ArrayList&lt;Integer&gt; lesser = new ArrayList&lt;Integer&gt;();_x000D_
+        ArrayList&lt;Integer&gt; greater = new ArrayList&lt;Integer&gt;();_x000D_
+_x000D_
+        for (Integer x : arr.subList(1, arr.size())) {_x000D_
+            if (x &lt; pivot) {_x000D_
+                lesser.add(x);_x000D_
+            } else if (x &gt;= pivot) {_x000D_
+                greater.add(x);_x000D_
+            }_x000D_
+        }_x000D_
+        ArrayList&lt;Integer&gt; middle = new ArrayList&lt;Integer&gt;();_x000D_
+        middle.add(pivot);_x000D_
+        lesser = quicksort(lesser);_x000D_
+        greater = quicksort(greater);_x000D_
+        middle.addAll(greater);_x000D_
+        lesser.addAll(middle);_x000D_
+        return lesser;_x000D_
+_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>} else if (x &gt; pivot) {</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+import java_programs.Node;
+public class REVERSE_LINKED_LIST {
+    public static Node reverse_linked_list(Node node) {
+        Node prevnode = null;
+        Node nextnode;
+        while (node != null) {
+            nextnode = node.getSuccessor();
+            node.setSuccessor(prevnode);
+            prevnode = node;
+            node = nextnode;
+        }
+        return prevnode;
+    }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Omission between the lines:  'node.setSuccessor(prevnode);' and 'node=nextnode;'
+while (node != null) {
+            nextnode = node.getSuccessor();
+            node.setSuccessor(prevnode);
+            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prevnode = node;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+            node = nextnode;
+        }
+        return prevnode;
+    }
+}                   </t>
+    </r>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+import java.util.function.BinaryOperator;
+public class RPN_EVAL {
+    public static Double rpn_eval(ArrayList tokens) {
+        Map&lt;String, BinaryOperator&lt;Double&gt;&gt; op = new HashMap&lt;String, BinaryOperator&lt;Double&gt;&gt;();
+        op.put("+", (a, b) -&gt; a + b);
+        op.put("-", (a, b) -&gt; a - b);
+        op.put("*", (a, b) -&gt; a * b);
+        op.put("/", (a, b) -&gt; a / b);
+        Stack stack = new Stack();
+        for (Object token : tokens) {
+            if (Double.class.isInstance(token)) {
+                stack.push((Double) token);
+            } else {
+                token = (String) token;
+                Double a = (Double) stack.pop();
+                Double b = (Double) stack.pop();
+                Double c = 0.0;
+                BinaryOperator&lt;Double&gt; bin_op = op.get(token);
+                c = bin_op.apply(b,a);
+                stack.push(c);
+            }
+        }
+        return (Double) stack.pop();
+    }
+}</t>
+  </si>
+  <si>
+    <t>c = bin_op.apply(a,b);</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+import java_programs.Node;
+import java_programs.WeightedEdge;
+import java.lang.Math.*;
+public class SHORTEST_PATHS {
+    final static int INF = 99999;
+    public static Map&lt;String, Integer&gt; shortest_paths(String source, Map&lt;List&lt;String&gt;,Integer&gt; weight_by_edge) {
+        Map&lt;String,Integer&gt; weight_by_node = new HashMap&lt;String,Integer&gt;();
+        for (List&lt;String&gt; edge : weight_by_edge.keySet()) {
+                weight_by_node.put(edge.get(1), INF);
+                weight_by_node.put(edge.get(0), INF);
+        }
+        weight_by_node.put(source, 0);
+        for (int i = 0; i &lt; weight_by_node.size(); i++) {
+            for (List&lt;String&gt; edge : weight_by_edge.keySet()) {
+                int update_weight = Math.min(
+                        weight_by_node.get(edge.get(0))
+                                + weight_by_edge.get(edge),
+                        weight_by_node.get(edge.get(1)));
+                weight_by_node.put(edge.get(1), update_weight);
+            }
+        }
+        return weight_by_node;
+    }
+}</t>
+  </si>
+  <si>
+    <t>weight_by_edge.put(edge, update_weight);</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+import java_programs.Node;
+public class SHORTEST_PATH_LENGTH {
+    public static int shortest_path_length(Map&lt;List&lt;Node&gt;, Integer&gt; length_by_edge, Node startnode, Node goalnode) {
+        int n = length_by_edge.size();
+        Map&lt;Node, Integer&gt; unvisitedNodes = new HashMap&lt;&gt;();
+        Set&lt;Node&gt; visitedNodes = new HashSet&lt;&gt;();
+        unvisitedNodes.put(startnode, 0);
+        while (!unvisitedNodes.isEmpty()) {
+            Node node = getNodeWithMinDistance(unvisitedNodes);
+            int distance = unvisitedNodes.get(node);
+            unvisitedNodes.remove(node);
+            if (node.getValue() == goalnode.getValue()) {
+                return distance;
+            }
+            visitedNodes.add(node);
+            for (Node nextnode : node.getSuccessors()) {
+                if (visitedNodes.contains(nextnode)) {
+                    continue;
+                }
+                if (unvisitedNodes.get(nextnode) == null) {
+                    unvisitedNodes.put(nextnode, Integer.MAX_VALUE);
+                }
+                unvisitedNodes.put(nextnode, Math.min(unvisitedNodes.get(nextnode),
+                        distance + length_by_edge.get(Arrays.asList(node, nextnode))));
+            }
+        }
+        return Integer.MAX_VALUE;
+    }
+    public static Node getNodeWithMinDistance(Map&lt;Node,Integer&gt; list) {
+        Node minNode = null;
+        int minDistance = Integer.MAX_VALUE;
+        for (Node node : list.keySet()) {
+            int distance = list.get(node);
+            if (distance &lt; minDistance) {
+                minDistance = distance;
+                minNode = node;
+            }
+        }
+        return minNode;
+    }
+}</t>
+  </si>
+  <si>
+    <t>unvisitedNodes.get(nextnode) + length_by_edge.get(Arrays.asList(node, nextnode))));</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+import java.lang.Math.*;
+public class SHORTEST_PATH_LENGTHS {
+    final static int INF = 99999;
+    public static Map&lt;List&lt;Integer&gt;,Integer&gt; shortest_path_lengths(int numNodes, Map&lt;List&lt;Integer&gt;,Integer&gt; length_by_edge) {
+        Map&lt;List&lt;Integer&gt;,Integer&gt; length_by_path = new HashMap&lt;&gt;();
+        for (int i = 0; i &lt; numNodes; i++) {
+            for (int j =0; j &lt; numNodes; j++) {
+                List&lt;Integer&gt; edge = new ArrayList&lt;&gt;(Arrays.asList(i,j));
+                if (i == j) {
+                    length_by_path.put(edge, 0);
+                }
+                else if (length_by_edge.containsKey(edge) ) {
+                    length_by_path.put(edge, length_by_edge.get(edge));
+                } else {
+                    length_by_path.put(edge, INF);
+                }
+            }
+        }
+        for (int k = 0; k &lt; numNodes; k++) {
+            for (int i = 0; i &lt; numNodes; i++) {
+                for (int j = 0; j &lt; numNodes; j++) {
+                    int update_length = Math.min(length_by_path.get(Arrays.asList(i,j)),
+                                                 sumLengths(length_by_path.get(Arrays.asList(i,k)),
+                                                            length_by_path.get(Arrays.asList(k,j))));
+                    length_by_path.put(Arrays.asList(i,j), update_length);
+                }
+            }
+        }
+        return length_by_path;
+    }
+    static private int sumLengths(int a, int b) {
+        if(a == INF || b == INF) {
+            return INF;
+        }
+        return a + b;
+    }
+}</t>
+  </si>
+  <si>
+    <t>length_by_path.get(Arrays.asList(j,k))));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">package correct_java_programs;
+import java.util.*;
+public class SHUNTING_YARD {
+    public static List shunting_yard(ArrayList tokens) {
+        Map&lt;String, Integer&gt; precedence = new HashMap&lt;String, Integer&gt;();
+        precedence.put("+", 1);
+        precedence.put("-", 1);
+        precedence.put("*", 2);
+        precedence.put("/", 2);
+        ArrayList rpntokens = new ArrayList(100);
+        ArrayDeque opstack = new ArrayDeque();
+        for (Object token : tokens) {
+            if (Integer.class.isInstance(token)) {
+                rpntokens.add((Integer) token);
+            } else {
+                String operator = (String) token;
+                while (!opstack.isEmpty() &amp;&amp; precedence.get(operator) &lt;= precedence.get(opstack.getLast())) {
+                    rpntokens.add(opstack.pop());
+                }
+                opstack.push(token);
+            }
+        }
+        while (!opstack.isEmpty()) {
+            rpntokens.add(opstack.pop());
+        }
+        return rpntokens;
+    }
+}
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Omission
+} else {
+                String operator = (String) token;
+                while (!opstack.isEmpty() &amp;&amp; precedence.get(operator) &lt;= precedence.get(opstack.getLast())) {
+                    rpntokens.add(opstack.pop());
+                }
+                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>opstack.push(token);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+            }
+        }</t>
+    </r>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+public class SIEVE {
+    public static boolean all(ArrayList&lt;Boolean&gt; arr) {
+        for (boolean value : arr) {
+            if (!value) { return false; }
+        }
+        return true;
+    }
+    public static boolean any(ArrayList&lt;Boolean&gt; arr) {
+        for (boolean value: arr) {
+            if (value) { return true; }
+        }
+        return false;
+    }
+    public static ArrayList&lt;Boolean&gt; list_comp(int n, ArrayList&lt;Integer&gt; primes) {
+        ArrayList&lt;Boolean&gt; built_comprehension = new ArrayList&lt;Boolean&gt;();
+        for (Integer p : primes) {
+            built_comprehension.add(n % p &gt; 0);
+        }
+        return built_comprehension;
+    }
+    public static ArrayList&lt;Integer&gt; sieve(Integer max) {
+        ArrayList&lt;Integer&gt; primes = new ArrayList&lt;Integer&gt;();
+        for (int n=2; n&lt;max+1; n++) {
+            if (all(list_comp(n, primes))) {
+                primes.add(n);
+            }
+        }
+        return primes;
+    }
+}</t>
+  </si>
+  <si>
+    <t>if (any(list_comp(n, primes))) {</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class SQRT {_x000D_
+    public static double sqrt(double x, double epsilon) {_x000D_
+        double approx = x / 2d;_x000D_
+        while (Math.abs(x-approx*approx) &gt; epsilon) {_x000D_
+            approx = 0.5d * (approx + x / approx);_x000D_
+        }_x000D_
+        return approx;_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>while (Math.abs(x-approx) &gt; epsilon) {</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+public class SUBSEQUENCES {
+    public static ArrayList&lt;ArrayList&gt; subsequences(int a, int b, int k) {
+        if (k == 0) {
+            ArrayList empty_set = new ArrayList&lt;ArrayList&gt;();
+            empty_set.add(new ArrayList());
+            return empty_set;
+        }
+        ArrayList ret = new ArrayList(50);
+        for (int i=a; i&lt;b+1-k; i++) {
+            ArrayList base = new ArrayList(50);
+            for (ArrayList rest : subsequences(i+1, b, k-1)) {
+                rest.add(0,i);
+                base.add(rest);
+            }
+            ret.addAll(base);
+        }
+        return ret;
+    }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if (k == 0) {
+            return new ArrayList();
+        }
+</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+import java_programs.Node;_x000D_
+_x000D_
+public class TOPOLOGICAL_ORDERING {_x000D_
+    public static ArrayList&lt;Node&gt; topological_ordering (List&lt;Node&gt; directedGraph) {_x000D_
+        ArrayList&lt;Node&gt; orderedNodes = new ArrayList&lt;Node&gt;();_x000D_
+        for (Node node : directedGraph) {_x000D_
+            if (node.getPredecessors().isEmpty()) {_x000D_
+                orderedNodes.add(node);_x000D_
+            }_x000D_
+        }_x000D_
+_x000D_
+        int listSize = orderedNodes.size();_x000D_
+        for (int i = 0; i &lt; listSize; i++) {_x000D_
+            Node node = orderedNodes.get(i);_x000D_
+            for (Node nextNode : node.getSuccessors()) {_x000D_
+                if (orderedNodes.containsAll(nextNode.getPredecessors()) &amp;&amp; !orderedNodes.contains(nextNode)) {_x000D_
+                    orderedNodes.add(nextNode);_x000D_
+                    listSize++;_x000D_
+                }_x000D_
+            }_x000D_
+        }_x000D_
+        return orderedNodes;_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>if (orderedNodes.containsAll(nextNode.getSuccessors()) &amp;&amp; !orderedNodes.contains(nextNode)) {</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;_x000D_
+import java.util.*;_x000D_
+_x000D_
+_x000D_
+public class TO_BASE {_x000D_
+    public static String to_base(int num, int b) {_x000D_
+        String result = "";_x000D_
+        String alphabet = "0123456789ABCDEFGHIJKLMNOPQRSTUVWXYZ";_x000D_
+        int i;_x000D_
+        while (num &gt; 0) {_x000D_
+            i = num % b;_x000D_
+            num = num / b; // floor division?_x000D_
+            result = String.valueOf(alphabet.charAt(i))+result;_x000D_
+        }_x000D_
+_x000D_
+        return result;_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>result = result + String.valueOf(alphabet.charAt(i));</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+public class WRAP {
+    public static void main(String[] args) {
+        System.out.println("abc".lastIndexOf("c",30));
+    }
+    public static ArrayList&lt;String&gt; wrap(String text, int cols) {
+        ArrayList&lt;String&gt; lines = new ArrayList&lt;String&gt;();
+        String line;
+        while (text.length() &gt; cols) {
+            int end = text.lastIndexOf(" ", cols); // off by one?
+            if (end == -1) {
+                end = cols;
+            }
+            line = text.substring(0,end);
+            text = text.substring(end);
+            lines.add(line);
+        }
+        lines.add(text);
+        return lines;
+    }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Omission - Before final return statement
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lines.add(text);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+        return lines;</t>
+    </r>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -4022,20 +5533,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="51.5546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4057,8 +5577,20 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -4069,10 +5601,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="1">
-        <v>225.0</v>
+        <v>225</v>
       </c>
       <c r="E2" s="1">
-        <v>129.0</v>
+        <v>129</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -4080,8 +5612,15 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="J2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -4092,10 +5631,10 @@
         <v>14</v>
       </c>
       <c r="D3" s="1">
-        <v>305.0</v>
+        <v>305</v>
       </c>
       <c r="E3" s="1">
-        <v>196.0</v>
+        <v>196</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>15</v>
@@ -4103,8 +5642,15 @@
       <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="H3" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -4115,10 +5661,10 @@
         <v>19</v>
       </c>
       <c r="D4" s="1">
-        <v>309.0</v>
+        <v>309</v>
       </c>
       <c r="E4" s="1">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>20</v>
@@ -4126,8 +5672,15 @@
       <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="J4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -4138,10 +5691,10 @@
         <v>24</v>
       </c>
       <c r="D5" s="1">
-        <v>319.0</v>
+        <v>319</v>
       </c>
       <c r="E5" s="1">
-        <v>205.0</v>
+        <v>205</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>25</v>
@@ -4149,8 +5702,15 @@
       <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H5" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="J5" s="2"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -4161,10 +5721,10 @@
         <v>29</v>
       </c>
       <c r="D6" s="1">
-        <v>258.0</v>
+        <v>258</v>
       </c>
       <c r="E6" s="1">
-        <v>158.0</v>
+        <v>158</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>30</v>
@@ -4172,8 +5732,15 @@
       <c r="G6" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="H6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="J6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -4184,10 +5751,10 @@
         <v>34</v>
       </c>
       <c r="D7" s="1">
-        <v>339.0</v>
+        <v>339</v>
       </c>
       <c r="E7" s="1">
-        <v>167.0</v>
+        <v>167</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>35</v>
@@ -4195,8 +5762,15 @@
       <c r="G7" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="H7" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -4207,10 +5781,10 @@
         <v>39</v>
       </c>
       <c r="D8" s="1">
-        <v>347.0</v>
+        <v>347</v>
       </c>
       <c r="E8" s="1">
-        <v>219.0</v>
+        <v>219</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>40</v>
@@ -4218,8 +5792,15 @@
       <c r="G8" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="H8" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -4230,10 +5811,10 @@
         <v>44</v>
       </c>
       <c r="D9" s="1">
-        <v>315.0</v>
+        <v>315</v>
       </c>
       <c r="E9" s="1">
-        <v>179.0</v>
+        <v>179</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>45</v>
@@ -4241,8 +5822,16 @@
       <c r="G9" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="H9" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -4253,10 +5842,10 @@
         <v>49</v>
       </c>
       <c r="D10" s="1">
-        <v>234.0</v>
+        <v>234</v>
       </c>
       <c r="E10" s="1">
-        <v>107.0</v>
+        <v>107</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>50</v>
@@ -4264,8 +5853,15 @@
       <c r="G10" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="H10" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J10" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -4276,10 +5872,10 @@
         <v>54</v>
       </c>
       <c r="D11" s="1">
-        <v>323.0</v>
+        <v>323</v>
       </c>
       <c r="E11" s="1">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>55</v>
@@ -4287,8 +5883,16 @@
       <c r="G11" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="H11" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>57</v>
       </c>
@@ -4299,10 +5903,10 @@
         <v>59</v>
       </c>
       <c r="D12" s="1">
-        <v>631.0</v>
+        <v>631</v>
       </c>
       <c r="E12" s="1">
-        <v>86.0</v>
+        <v>86</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>60</v>
@@ -4310,8 +5914,15 @@
       <c r="G12" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="H12" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="J12" s="2"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -4322,10 +5933,10 @@
         <v>64</v>
       </c>
       <c r="D13" s="1">
-        <v>286.0</v>
+        <v>286</v>
       </c>
       <c r="E13" s="1">
-        <v>165.0</v>
+        <v>165</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>65</v>
@@ -4333,8 +5944,15 @@
       <c r="G13" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="H13" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
@@ -4345,10 +5963,10 @@
         <v>69</v>
       </c>
       <c r="D14" s="1">
-        <v>467.0</v>
+        <v>467</v>
       </c>
       <c r="E14" s="1">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>70</v>
@@ -4356,8 +5974,15 @@
       <c r="G14" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="H14" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="J14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -4368,10 +5993,10 @@
         <v>74</v>
       </c>
       <c r="D15" s="1">
-        <v>522.0</v>
+        <v>522</v>
       </c>
       <c r="E15" s="1">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>75</v>
@@ -4379,8 +6004,15 @@
       <c r="G15" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="H15" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="J15" s="2"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
@@ -4391,10 +6023,10 @@
         <v>79</v>
       </c>
       <c r="D16" s="1">
-        <v>349.0</v>
+        <v>349</v>
       </c>
       <c r="E16" s="1">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>80</v>
@@ -4402,8 +6034,15 @@
       <c r="G16" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="H16" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="J16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
@@ -4414,10 +6053,10 @@
         <v>84</v>
       </c>
       <c r="D17" s="1">
-        <v>534.0</v>
+        <v>534</v>
       </c>
       <c r="E17" s="1">
-        <v>459.0</v>
+        <v>459</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>85</v>
@@ -4425,8 +6064,16 @@
       <c r="G17" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="H17" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>87</v>
       </c>
@@ -4437,10 +6084,10 @@
         <v>89</v>
       </c>
       <c r="D18" s="1">
-        <v>408.0</v>
+        <v>408</v>
       </c>
       <c r="E18" s="1">
-        <v>206.0</v>
+        <v>206</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>90</v>
@@ -4448,8 +6095,15 @@
       <c r="G18" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="H18" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J18" s="2"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>92</v>
       </c>
@@ -4460,10 +6114,10 @@
         <v>94</v>
       </c>
       <c r="D19" s="1">
-        <v>369.0</v>
+        <v>369</v>
       </c>
       <c r="E19" s="1">
-        <v>260.0</v>
+        <v>260</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>95</v>
@@ -4471,8 +6125,16 @@
       <c r="G19" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="H19" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>97</v>
       </c>
@@ -4483,10 +6145,10 @@
         <v>99</v>
       </c>
       <c r="D20" s="1">
-        <v>375.0</v>
+        <v>375</v>
       </c>
       <c r="E20" s="1">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>100</v>
@@ -4494,8 +6156,16 @@
       <c r="G20" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="H20" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>102</v>
       </c>
@@ -4506,10 +6176,10 @@
         <v>104</v>
       </c>
       <c r="D21" s="1">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="E21" s="1">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>105</v>
@@ -4517,8 +6187,16 @@
       <c r="G21" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="H21" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>107</v>
       </c>
@@ -4529,10 +6207,10 @@
         <v>109</v>
       </c>
       <c r="D22" s="1">
-        <v>422.0</v>
+        <v>422</v>
       </c>
       <c r="E22" s="1">
-        <v>165.0</v>
+        <v>165</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>110</v>
@@ -4540,8 +6218,15 @@
       <c r="G22" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="H22" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="J22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>112</v>
       </c>
@@ -4552,10 +6237,10 @@
         <v>114</v>
       </c>
       <c r="D23" s="1">
-        <v>578.0</v>
+        <v>578</v>
       </c>
       <c r="E23" s="1">
-        <v>405.0</v>
+        <v>405</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>115</v>
@@ -4563,8 +6248,16 @@
       <c r="G23" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="H23" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="6"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>117</v>
       </c>
@@ -4575,10 +6268,10 @@
         <v>119</v>
       </c>
       <c r="D24" s="1">
-        <v>448.0</v>
+        <v>448</v>
       </c>
       <c r="E24" s="1">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>120</v>
@@ -4586,8 +6279,16 @@
       <c r="G24" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="H24" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="J24" s="5"/>
+      <c r="K24" s="6"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>122</v>
       </c>
@@ -4598,16 +6299,24 @@
         <v>124</v>
       </c>
       <c r="D25" s="1">
-        <v>425.0</v>
+        <v>425</v>
       </c>
       <c r="E25" s="1">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="H25" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="J25" s="5"/>
+      <c r="K25" s="6"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>126</v>
       </c>
@@ -4618,10 +6327,10 @@
         <v>128</v>
       </c>
       <c r="D26" s="1">
-        <v>438.0</v>
+        <v>438</v>
       </c>
       <c r="E26" s="1">
-        <v>371.0</v>
+        <v>371</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>129</v>
@@ -4629,8 +6338,13 @@
       <c r="G26" s="1" t="s">
         <v>130</v>
       </c>
+      <c r="H26" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="I26" s="7"/>
+      <c r="J26" s="2"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>131</v>
       </c>
@@ -4641,10 +6355,10 @@
         <v>133</v>
       </c>
       <c r="D27" s="1">
-        <v>418.0</v>
+        <v>418</v>
       </c>
       <c r="E27" s="1">
-        <v>274.0</v>
+        <v>274</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>134</v>
@@ -4652,8 +6366,16 @@
       <c r="G27" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="H27" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="J27" s="5"/>
+      <c r="K27" s="6"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>136</v>
       </c>
@@ -4664,10 +6386,10 @@
         <v>138</v>
       </c>
       <c r="D28" s="1">
-        <v>427.0</v>
+        <v>427</v>
       </c>
       <c r="E28" s="1">
-        <v>176.0</v>
+        <v>176</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>139</v>
@@ -4675,8 +6397,16 @@
       <c r="G28" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="H28" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="J28" s="5"/>
+      <c r="K28" s="6"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>141</v>
       </c>
@@ -4687,10 +6417,10 @@
         <v>143</v>
       </c>
       <c r="D29" s="1">
-        <v>394.0</v>
+        <v>394</v>
       </c>
       <c r="E29" s="1">
-        <v>201.0</v>
+        <v>201</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>144</v>
@@ -4698,8 +6428,16 @@
       <c r="G29" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="H29" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>146</v>
       </c>
@@ -4710,16 +6448,24 @@
         <v>148</v>
       </c>
       <c r="D30" s="1">
-        <v>309.0</v>
+        <v>309</v>
       </c>
       <c r="E30" s="1">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="H30" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="6"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>150</v>
       </c>
@@ -4730,10 +6476,10 @@
         <v>152</v>
       </c>
       <c r="D31" s="1">
-        <v>312.0</v>
+        <v>312</v>
       </c>
       <c r="E31" s="1">
-        <v>174.0</v>
+        <v>174</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>153</v>
@@ -4741,8 +6487,15 @@
       <c r="G31" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="H31" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="J31" s="2"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>155</v>
       </c>
@@ -4753,10 +6506,10 @@
         <v>157</v>
       </c>
       <c r="D32" s="1">
-        <v>428.0</v>
+        <v>428</v>
       </c>
       <c r="E32" s="1">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>158</v>
@@ -4764,8 +6517,16 @@
       <c r="G32" s="1" t="s">
         <v>159</v>
       </c>
+      <c r="H32" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="6"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>160</v>
       </c>
@@ -4776,10 +6537,10 @@
         <v>162</v>
       </c>
       <c r="D33" s="1">
-        <v>733.0</v>
+        <v>733</v>
       </c>
       <c r="E33" s="1">
-        <v>146.0</v>
+        <v>146</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>163</v>
@@ -4787,8 +6548,15 @@
       <c r="G33" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="H33" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="J33" s="2"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>165</v>
       </c>
@@ -4799,10 +6567,10 @@
         <v>167</v>
       </c>
       <c r="D34" s="1">
-        <v>560.0</v>
+        <v>560</v>
       </c>
       <c r="E34" s="1">
-        <v>87.0</v>
+        <v>87</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>168</v>
@@ -4810,8 +6578,15 @@
       <c r="G34" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="H34" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="J34" s="2"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>170</v>
       </c>
@@ -4822,10 +6597,10 @@
         <v>172</v>
       </c>
       <c r="D35" s="1">
-        <v>571.0</v>
+        <v>571</v>
       </c>
       <c r="E35" s="1">
-        <v>439.0</v>
+        <v>439</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>173</v>
@@ -4833,8 +6608,15 @@
       <c r="G35" s="1" t="s">
         <v>174</v>
       </c>
+      <c r="H35" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J35" s="2"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>175</v>
       </c>
@@ -4845,10 +6627,10 @@
         <v>177</v>
       </c>
       <c r="D36" s="1">
-        <v>537.0</v>
+        <v>537</v>
       </c>
       <c r="E36" s="1">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>178</v>
@@ -4856,8 +6638,16 @@
       <c r="G36" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="H36" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36" s="6"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>180</v>
       </c>
@@ -4868,10 +6658,10 @@
         <v>182</v>
       </c>
       <c r="D37" s="1">
-        <v>373.0</v>
+        <v>373</v>
       </c>
       <c r="E37" s="1">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>183</v>
@@ -4879,8 +6669,15 @@
       <c r="G37" s="1" t="s">
         <v>184</v>
       </c>
+      <c r="H37" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="J37" s="2"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>185</v>
       </c>
@@ -4891,10 +6688,10 @@
         <v>187</v>
       </c>
       <c r="D38" s="1">
-        <v>269.0</v>
+        <v>269</v>
       </c>
       <c r="E38" s="1">
-        <v>144.0</v>
+        <v>144</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>188</v>
@@ -4902,8 +6699,15 @@
       <c r="G38" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="H38" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="J38" s="2"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>190</v>
       </c>
@@ -4914,10 +6718,10 @@
         <v>192</v>
       </c>
       <c r="D39" s="1">
-        <v>344.0</v>
+        <v>344</v>
       </c>
       <c r="E39" s="1">
-        <v>177.0</v>
+        <v>177</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>193</v>
@@ -4925,8 +6729,16 @@
       <c r="G39" s="1" t="s">
         <v>194</v>
       </c>
+      <c r="H39" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="J39" s="5"/>
+      <c r="K39" s="6"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>195</v>
       </c>
@@ -4937,10 +6749,10 @@
         <v>197</v>
       </c>
       <c r="D40" s="1">
-        <v>351.0</v>
+        <v>351</v>
       </c>
       <c r="E40" s="1">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>198</v>
@@ -4948,8 +6760,15 @@
       <c r="G40" s="1" t="s">
         <v>199</v>
       </c>
+      <c r="H40" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="J40" s="2"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>200</v>
       </c>
@@ -4960,10 +6779,10 @@
         <v>202</v>
       </c>
       <c r="D41" s="1">
-        <v>287.0</v>
+        <v>287</v>
       </c>
       <c r="E41" s="1">
-        <v>235.0</v>
+        <v>235</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>203</v>
@@ -4971,8 +6790,15 @@
       <c r="G41" s="1" t="s">
         <v>204</v>
       </c>
+      <c r="H41" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="J41" s="2"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>205</v>
       </c>
@@ -4983,10 +6809,10 @@
         <v>207</v>
       </c>
       <c r="D42" s="1">
-        <v>254.0</v>
+        <v>254</v>
       </c>
       <c r="E42" s="1">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>208</v>
@@ -4994,8 +6820,13 @@
       <c r="G42" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="H42" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="I42" s="7"/>
+      <c r="J42" s="2"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>210</v>
       </c>
@@ -5006,10 +6837,10 @@
         <v>212</v>
       </c>
       <c r="D43" s="1">
-        <v>399.0</v>
+        <v>399</v>
       </c>
       <c r="E43" s="1">
-        <v>205.0</v>
+        <v>205</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>213</v>
@@ -5017,8 +6848,45 @@
       <c r="G43" s="1" t="s">
         <v>214</v>
       </c>
+      <c r="H43" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="2"/>
+      <c r="I44" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" s="2">
+        <f>COUNTIF(J2:J43,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="2"/>
+      <c r="I45" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2">
+        <f>COUNTIF(J2:J43,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="2"/>
+      <c r="I46" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="J46" s="2" t="e">
+        <f>J44/(J44+J45)*100</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adjust: Rerun 3.5 Turbo QuixBugs Java Tests
</commit_message>
<xml_diff>
--- a/Analysis/QuixBugs_GPT_APR/APR_one_shot_ChatGPT_3.5_turbo_Java.xlsx
+++ b/Analysis/QuixBugs_GPT_APR/APR_one_shot_ChatGPT_3.5_turbo_Java.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Investigation Proper\Bug-Busters\Analysis\QuixBugs_GPT_APR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21030CB-0324-47AC-8B3B-A9B9ED6DD1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11311D69-8483-4CF4-B92E-93BD9CE7FDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="318">
   <si>
     <t>File Name</t>
   </si>
@@ -3833,43 +3833,6 @@
     <t>n = (n ^ (n - 1));</t>
   </si>
   <si>
-    <t>package correct_java_programs;_x000D_
-import java.util.*;_x000D_
-import java.util.ArrayDeque;_x000D_
-_x000D_
-import java_programs.Node;_x000D_
-_x000D_
-_x000D_
-public class BREADTH_FIRST_SEARCH {_x000D_
-_x000D_
-    public static Set&lt;Node&gt; nodesvisited = new HashSet&lt;&gt;();_x000D_
-_x000D_
-    public static boolean breadth_first_search(Node startnode, Node goalnode) {_x000D_
-        Deque&lt;Node&gt; queue = new ArrayDeque&lt;&gt;();_x000D_
-        queue.addLast(startnode);_x000D_
-_x000D_
-        nodesvisited.add(startnode);_x000D_
-_x000D_
-        while (!queue.isEmpty()) {_x000D_
-            Node node = queue.removeFirst();_x000D_
-_x000D_
-            if (node == goalnode) {_x000D_
-                return true;_x000D_
-            } else {_x000D_
-                for (Node successor_node : node.getSuccessors()) {_x000D_
-                    if (!nodesvisited.contains(successor_node)) {_x000D_
-                        queue.addFirst(successor_node);_x000D_
-                        nodesvisited.add(successor_node);_x000D_
-                    }_x000D_
-                }_x000D_
-            }_x000D_
-        }_x000D_
-         return false;_x000D_
-    }_x000D_
-_x000D_
-}</t>
-  </si>
-  <si>
     <t>while (true) {</t>
   </si>
   <si>
@@ -5228,6 +5191,2502 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>package correct_java_programs;
+import java.util.*;
+import java.util.ArrayDeque;
+import java_programs.Node;
+public class BREADTH_FIRST_SEARCH {
+    public static Set&lt;Node&gt; nodesvisited = new HashSet&lt;&gt;();
+    public static boolean breadth_first_search(Node startnode, Node goalnode) {
+        Deque&lt;Node&gt; queue = new ArrayDeque&lt;&gt;();
+        queue.addLast(startnode);
+        nodesvisited.add(startnode);
+        while (!queue.isEmpty()) {
+            Node node = queue.removeFirst();
+            if (node == goalnode) {
+                return true;
+            } else {
+                for (Node successor_node : node.getSuccessors()) {
+                    if (!nodesvisited.contains(successor_node)) {
+                        queue.addFirst(successor_node);
+                        nodesvisited.add(successor_node);
+                    }
+                }
+            }
+        }
+         return false;
+    }
+}</t>
+  </si>
+  <si>
+    <t>Stack Overflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%TESTC  7 v2
+%TSTTREE1,java_testcases.junit.FIND_FIRST_IN_SORTED_TEST,true,7,false,-1,java_testcases.junit.FIND_FIRST_IN_SORTED_TEST,,
+%TSTTREE2,test_0(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),false,1,false,-1,test_0(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),,
+%TSTTREE3,test_1(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),false,1,false,-1,test_1(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),,
+%TSTTREE4,test_2(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),false,1,false,-1,test_2(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),,
+%TSTTREE5,test_3(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),false,1,false,-1,test_3(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),,
+%TSTTREE6,test_4(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),false,1,false,-1,test_4(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),,
+%TSTTREE7,test_5(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),false,1,false,-1,test_5(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),,
+%TSTTREE8,test_6(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),false,1,false,-1,test_6(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST),,
+%TESTS  2,test_0(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTE  2,test_0(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTS  3,test_1(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTE  3,test_1(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTS  4,test_2(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTE  4,test_2(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTS  5,test_3(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTE  5,test_3(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTS  6,test_4(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTE  6,test_4(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTS  7,test_5(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTE  7,test_5(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TESTS  8,test_6(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%FAILED 8,test_6(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%TRACES 
+java.lang.AssertionError: expected:&lt;7&gt; but was:&lt;-1&gt;
+        at org.junit.Assert.fail(Assert.java:89)
+        at org.junit.Assert.failNotEquals(Assert.java:835)
+        at org.junit.Assert.assertEquals(Assert.java:647)
+        at org.junit.Assert.assertEquals(Assert.java:633)
+        at java_testcases.junit.FIND_FIRST_IN_SORTED_TEST.test_6(FIND_FIRST_IN_SORTED_TEST.java:44)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  8,test_6(java_testcases.junit.FIND_FIRST_IN_SORTED_TEST)
+%RUNTIME128
+</t>
+  </si>
+  <si>
+    <t>%TESTC  11 v2
+%TSTTREE1,java_testcases.junit.GET_FACTORS_TEST,true,11,false,-1,java_testcases.junit.GET_FACTORS_TEST,,
+%TSTTREE2,test_10(java_testcases.junit.GET_FACTORS_TEST),false,1,false,-1,test_10(java_testcases.junit.GET_FACTORS_TEST),,
+%TSTTREE3,test_0(java_testcases.junit.GET_FACTORS_TEST),false,1,false,-1,test_0(java_testcases.junit.GET_FACTORS_TEST),,
+%TSTTREE4,test_1(java_testcases.junit.GET_FACTORS_TEST),false,1,false,-1,test_1(java_testcases.junit.GET_FACTORS_TEST),,
+%TSTTREE5,test_2(java_testcases.junit.GET_FACTORS_TEST),false,1,false,-1,test_2(java_testcases.junit.GET_FACTORS_TEST),,
+%TSTTREE6,test_3(java_testcases.junit.GET_FACTORS_TEST),false,1,false,-1,test_3(java_testcases.junit.GET_FACTORS_TEST),,
+%TSTTREE7,test_4(java_testcases.junit.GET_FACTORS_TEST),false,1,false,-1,test_4(java_testcases.junit.GET_FACTORS_TEST),,
+%TSTTREE8,test_5(java_testcases.junit.GET_FACTORS_TEST),false,1,false,-1,test_5(java_testcases.junit.GET_FACTORS_TEST),,
+%TSTTREE9,test_6(java_testcases.junit.GET_FACTORS_TEST),false,1,false,-1,test_6(java_testcases.junit.GET_FACTORS_TEST),,
+%TSTTREE10,test_7(java_testcases.junit.GET_FACTORS_TEST),false,1,false,-1,test_7(java_testcases.junit.GET_FACTORS_TEST),,
+%TSTTREE11,test_8(java_testcases.junit.GET_FACTORS_TEST),false,1,false,-1,test_8(java_testcases.junit.GET_FACTORS_TEST),,
+%TSTTREE12,test_9(java_testcases.junit.GET_FACTORS_TEST),false,1,false,-1,test_9(java_testcases.junit.GET_FACTORS_TEST),,
+%TESTS  2,test_10(java_testcases.junit.GET_FACTORS_TEST)
+%ERROR  2,test_10(java_testcases.junit.GET_FACTORS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Unreachable code
+        at java_programs.GET_FACTORS.get_factors(GET_FACTORS.java:15)
+        at java_testcases.junit.GET_FACTORS_TEST.test_10(GET_FACTORS_TEST.java:77)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  2,test_10(java_testcases.junit.GET_FACTORS_TEST)
+%TESTS  3,test_0(java_testcases.junit.GET_FACTORS_TEST)
+%ERROR  3,test_0(java_testcases.junit.GET_FACTORS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Unreachable code
+        at java_programs.GET_FACTORS.get_factors(GET_FACTORS.java:15)
+        at java_testcases.junit.GET_FACTORS_TEST.test_0(GET_FACTORS_TEST.java:7)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  3,test_0(java_testcases.junit.GET_FACTORS_TEST)
+%TESTS  4,test_1(java_testcases.junit.GET_FACTORS_TEST)
+%ERROR  4,test_1(java_testcases.junit.GET_FACTORS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Unreachable code
+        at java_programs.GET_FACTORS.get_factors(GET_FACTORS.java:15)
+        at java_testcases.junit.GET_FACTORS_TEST.test_1(GET_FACTORS_TEST.java:14)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  4,test_1(java_testcases.junit.GET_FACTORS_TEST)
+%TESTS  5,test_2(java_testcases.junit.GET_FACTORS_TEST)
+%ERROR  5,test_2(java_testcases.junit.GET_FACTORS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Unreachable code
+        at java_programs.GET_FACTORS.get_factors(GET_FACTORS.java:15)
+        at java_testcases.junit.GET_FACTORS_TEST.test_2(GET_FACTORS_TEST.java:21)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  5,test_2(java_testcases.junit.GET_FACTORS_TEST)
+%TESTS  6,test_3(java_testcases.junit.GET_FACTORS_TEST)
+%ERROR  6,test_3(java_testcases.junit.GET_FACTORS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Unreachable code
+        at java_programs.GET_FACTORS.get_factors(GET_FACTORS.java:15)
+        at java_testcases.junit.GET_FACTORS_TEST.test_3(GET_FACTORS_TEST.java:28)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  6,test_3(java_testcases.junit.GET_FACTORS_TEST)
+%TESTS  7,test_4(java_testcases.junit.GET_FACTORS_TEST)
+%ERROR  7,test_4(java_testcases.junit.GET_FACTORS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Unreachable code
+        at java_programs.GET_FACTORS.get_factors(GET_FACTORS.java:15)
+        at java_testcases.junit.GET_FACTORS_TEST.test_4(GET_FACTORS_TEST.java:35)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  7,test_4(java_testcases.junit.GET_FACTORS_TEST)
+%TESTS  8,test_5(java_testcases.junit.GET_FACTORS_TEST)
+%ERROR  8,test_5(java_testcases.junit.GET_FACTORS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Unreachable code
+        at java_programs.GET_FACTORS.get_factors(GET_FACTORS.java:15)
+        at java_testcases.junit.GET_FACTORS_TEST.test_5(GET_FACTORS_TEST.java:42)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  8,test_5(java_testcases.junit.GET_FACTORS_TEST)
+%TESTS  9,test_6(java_testcases.junit.GET_FACTORS_TEST)
+%ERROR  9,test_6(java_testcases.junit.GET_FACTORS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Unreachable code
+        at java_programs.GET_FACTORS.get_factors(GET_FACTORS.java:15)
+        at java_testcases.junit.GET_FACTORS_TEST.test_6(GET_FACTORS_TEST.java:49)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  9,test_6(java_testcases.junit.GET_FACTORS_TEST)
+%TESTS  10,test_7(java_testcases.junit.GET_FACTORS_TEST)
+%ERROR  10,test_7(java_testcases.junit.GET_FACTORS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Unreachable code
+        at java_programs.GET_FACTORS.get_factors(GET_FACTORS.java:15)
+        at java_testcases.junit.GET_FACTORS_TEST.test_7(GET_FACTORS_TEST.java:56)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  10,test_7(java_testcases.junit.GET_FACTORS_TEST)
+%TESTS  11,test_8(java_testcases.junit.GET_FACTORS_TEST)
+%ERROR  11,test_8(java_testcases.junit.GET_FACTORS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Unreachable code
+        at java_programs.GET_FACTORS.get_factors(GET_FACTORS.java:15)
+        at java_testcases.junit.GET_FACTORS_TEST.test_8(GET_FACTORS_TEST.java:63)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  11,test_8(java_testcases.junit.GET_FACTORS_TEST)
+%TESTS  12,test_9(java_testcases.junit.GET_FACTORS_TEST)
+%ERROR  12,test_9(java_testcases.junit.GET_FACTORS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Unreachable code
+        at java_programs.GET_FACTORS.get_factors(GET_FACTORS.java:15)
+        at java_testcases.junit.GET_FACTORS_TEST.test_9(GET_FACTORS_TEST.java:70)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  12,test_9(java_testcases.junit.GET_FACTORS_TEST)
+%RUNTIME172</t>
+  </si>
+  <si>
+    <t>%TESTC  7 v2
+%TSTTREE1,java_testcases.junit.HANOI_TEST,true,7,false,-1,java_testcases.junit.HANOI_TEST,,
+%TSTTREE2,test_0(java_testcases.junit.HANOI_TEST),false,1,false,-1,test_0(java_testcases.junit.HANOI_TEST),,
+%TSTTREE3,test_1(java_testcases.junit.HANOI_TEST),false,1,false,-1,test_1(java_testcases.junit.HANOI_TEST),,
+%TSTTREE4,test_2(java_testcases.junit.HANOI_TEST),false,1,false,-1,test_2(java_testcases.junit.HANOI_TEST),,
+%TSTTREE5,test_3(java_testcases.junit.HANOI_TEST),false,1,false,-1,test_3(java_testcases.junit.HANOI_TEST),,
+%TSTTREE6,test_4(java_testcases.junit.HANOI_TEST),false,1,false,-1,test_4(java_testcases.junit.HANOI_TEST),,
+%TSTTREE7,test_5(java_testcases.junit.HANOI_TEST),false,1,false,-1,test_5(java_testcases.junit.HANOI_TEST),,
+%TSTTREE8,test_6(java_testcases.junit.HANOI_TEST),false,1,false,-1,test_6(java_testcases.junit.HANOI_TEST),,
+%TESTS  2,test_0(java_testcases.junit.HANOI_TEST)
+%FAILED 2,test_0(java_testcases.junit.HANOI_TEST)
+%EXPECTS
+[[1,3]]
+%EXPECTE
+%ACTUALS
+[[1,2]]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[1,[3]]]&gt; but was:&lt;[[1,[2]]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.HANOI_TEST.test_0(HANOI_TEST.java:9)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  2,test_0(java_testcases.junit.HANOI_TEST)
+%TESTS  3,test_1(java_testcases.junit.HANOI_TEST)
+%FAILED 3,test_1(java_testcases.junit.HANOI_TEST)
+%EXPECTS
+[[1,2],[1,3],[2,3]]
+%EXPECTE
+%ACTUALS
+[[1,3],[1,2],[2,1]]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[1,[2],[1,3],[2,3]]]&gt; but was:&lt;[[1,[3],[1,2],[2,1]]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.HANOI_TEST.test_1(HANOI_TEST.java:16)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  3,test_1(java_testcases.junit.HANOI_TEST)
+%TESTS  4,test_2(java_testcases.junit.HANOI_TEST)
+%FAILED 4,test_2(java_testcases.junit.HANOI_TEST)
+%EXPECTS
+[[1,3],[1,2],[3,2],[1,3],[2,1],[2,3],[1,3]]
+%EXPECTE
+%ACTUALS
+[[1,2],[1,3],[3,1],[1,2],[2,3],[2,1],[1,2]]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[1,[3],[1,2],[3,2],[1,3],[2,1],[2,3],[1,3]]]&gt; but was:&lt;[[1,[2],[1,3],[3,1],[1,2],[2,3],[2,1],[1,2]]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.HANOI_TEST.test_2(HANOI_TEST.java:23)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  4,test_2(java_testcases.junit.HANOI_TEST)
+%TESTS  5,test_3(java_testcases.junit.HANOI_TEST)
+%FAILED 5,test_3(java_testcases.junit.HANOI_TEST)
+%EXPECTS
+[[1,2],[1,3],[2,3],[1,2],[3,1],[3,2],[1,2],[1,3],[2,3],[2,1],[3,1],[2,3],[1,2],[1,3],[2,3]]
+%EXPECTE
+%ACTUALS
+[[1,3],[1,2],[2,1],[1,3],[3,2],[3,1],[1,3],[1,2],[2,1],[2,3],[3,2],[2,1],[1,3],[1,2],[2,1]]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[1,[2],[1,3],[2,3],[1,2],[3,1],[3,2],[1,2],[1,3],[2,3],[2,1],[3,1],[2,3],[1,2],[1,3],[2,3]]]&gt; but was:&lt;[[1,[3],[1,2],[2,1],[1,3],[3,2],[3,1],[1,3],[1,2],[2,1],[2,3],[3,2],[2,1],[1,3],[1,2],[2,1]]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.HANOI_TEST.test_3(HANOI_TEST.java:30)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  5,test_3(java_testcases.junit.HANOI_TEST)
+%TESTS  6,test_4(java_testcases.junit.HANOI_TEST)
+%FAILED 6,test_4(java_testcases.junit.HANOI_TEST)
+%EXPECTS
+[[1,3],[1,2],[3,2]]
+%EXPECTE
+%ACTUALS
+[[1,2],[1,3],[3,1]]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[1,[3],[1,2],[3,2]]]&gt; but was:&lt;[[1,[2],[1,3],[3,1]]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.HANOI_TEST.test_4(HANOI_TEST.java:37)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  6,test_4(java_testcases.junit.HANOI_TEST)
+%TESTS  7,test_5(java_testcases.junit.HANOI_TEST)
+%FAILED 7,test_5(java_testcases.junit.HANOI_TEST)
+%EXPECTS
+[[1,2],[1,1],[2,1]]
+%EXPECTE
+%ACTUALS
+[[1,3],[1,2],[2,3]]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[1,[2],[1,1],[2,1]]]&gt; but was:&lt;[[1,[3],[1,2],[2,3]]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.HANOI_TEST.test_5(HANOI_TEST.java:44)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  7,test_5(java_testcases.junit.HANOI_TEST)
+%TESTS  8,test_6(java_testcases.junit.HANOI_TEST)
+%FAILED 8,test_6(java_testcases.junit.HANOI_TEST)
+%EXPECTS
+[[3,2],[3,1],[2,1]]
+%EXPECTE
+%ACTUALS
+[[3,1],[3,2],[2,3]]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[3,[2],[3,1],[2,1]]]&gt; but was:&lt;[[3,[1],[3,2],[2,3]]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.HANOI_TEST.test_6(HANOI_TEST.java:51)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  8,test_6(java_testcases.junit.HANOI_TEST)
+%RUNTIME321</t>
+  </si>
+  <si>
+    <t>%TESTC  7 v2
+%TSTTREE1,java_testcases.junit.KTH_TEST,true,7,false,-1,java_testcases.junit.KTH_TEST,,
+%TSTTREE2,test_0(java_testcases.junit.KTH_TEST),false,1,false,-1,test_0(java_testcases.junit.KTH_TEST),,
+%TSTTREE3,test_1(java_testcases.junit.KTH_TEST),false,1,false,-1,test_1(java_testcases.junit.KTH_TEST),,
+%TSTTREE4,test_2(java_testcases.junit.KTH_TEST),false,1,false,-1,test_2(java_testcases.junit.KTH_TEST),,
+%TSTTREE5,test_3(java_testcases.junit.KTH_TEST),false,1,false,-1,test_3(java_testcases.junit.KTH_TEST),,
+%TSTTREE6,test_4(java_testcases.junit.KTH_TEST),false,1,false,-1,test_4(java_testcases.junit.KTH_TEST),,
+%TSTTREE7,test_5(java_testcases.junit.KTH_TEST),false,1,false,-1,test_5(java_testcases.junit.KTH_TEST),,
+%TSTTREE8,test_6(java_testcases.junit.KTH_TEST),false,1,false,-1,test_6(java_testcases.junit.KTH_TEST),,
+%TESTS  2,test_0(java_testcases.junit.KTH_TEST)
+%ERROR  2,test_0(java_testcases.junit.KTH_TEST)
+%TRACES 
+java.lang.IndexOutOfBoundsException: Index 0 out of bounds for length 0
+        at java.base/jdk.internal.util.Preconditions.outOfBounds(Preconditions.java:64)
+        at java.base/jdk.internal.util.Preconditions.outOfBoundsCheckIndex(Preconditions.java:70)
+        at java.base/jdk.internal.util.Preconditions.checkIndex(Preconditions.java:248)
+        at java.base/java.util.Objects.checkIndex(Objects.java:372)
+        at java.base/java.util.ArrayList.get(ArrayList.java:459)
+        at java_programs.KTH.kth(KTH.java:5)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_testcases.junit.KTH_TEST.test_0(KTH_TEST.java:7)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  2,test_0(java_testcases.junit.KTH_TEST)
+%TESTS  3,test_1(java_testcases.junit.KTH_TEST)
+%ERROR  3,test_1(java_testcases.junit.KTH_TEST)
+%TRACES 
+java.lang.IndexOutOfBoundsException: Index 0 out of bounds for length 0
+        at java.base/jdk.internal.util.Preconditions.outOfBounds(Preconditions.java:64)
+        at java.base/jdk.internal.util.Preconditions.outOfBoundsCheckIndex(Preconditions.java:70)
+        at java.base/jdk.internal.util.Preconditions.checkIndex(Preconditions.java:248)
+        at java.base/java.util.Objects.checkIndex(Objects.java:372)
+        at java.base/java.util.ArrayList.get(ArrayList.java:459)
+        at java_programs.KTH.kth(KTH.java:5)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_testcases.junit.KTH_TEST.test_1(KTH_TEST.java:13)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  3,test_1(java_testcases.junit.KTH_TEST)
+%TESTS  4,test_2(java_testcases.junit.KTH_TEST)
+%TESTE  4,test_2(java_testcases.junit.KTH_TEST)
+%TESTS  5,test_3(java_testcases.junit.KTH_TEST)
+%TESTE  5,test_3(java_testcases.junit.KTH_TEST)
+%TESTS  6,test_4(java_testcases.junit.KTH_TEST)
+%TESTE  6,test_4(java_testcases.junit.KTH_TEST)
+%TESTS  7,test_5(java_testcases.junit.KTH_TEST)
+%ERROR  7,test_5(java_testcases.junit.KTH_TEST)
+%TRACES 
+java.lang.IndexOutOfBoundsException: Index 0 out of bounds for length 0
+        at java.base/jdk.internal.util.Preconditions.outOfBounds(Preconditions.java:64)
+        at java.base/jdk.internal.util.Preconditions.outOfBoundsCheckIndex(Preconditions.java:70)
+        at java.base/jdk.internal.util.Preconditions.checkIndex(Preconditions.java:248)
+        at java.base/java.util.Objects.checkIndex(Objects.java:372)
+        at java.base/java.util.ArrayList.get(ArrayList.java:459)
+        at java_programs.KTH.kth(KTH.java:5)
+        at java_programs.KTH.kth(KTH.java:20)
+        at java_programs.KTH.kth(KTH.java:20)
+        at java_programs.KTH.kth(KTH.java:20)
+        at java_testcases.junit.KTH_TEST.test_5(KTH_TEST.java:37)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  7,test_5(java_testcases.junit.KTH_TEST)
+%TESTS  8,test_6(java_testcases.junit.KTH_TEST)
+%ERROR  8,test_6(java_testcases.junit.KTH_TEST)
+%TRACES 
+java.lang.IndexOutOfBoundsException: Index 0 out of bounds for length 0
+        at java.base/jdk.internal.util.Preconditions.outOfBounds(Preconditions.java:64)
+        at java.base/jdk.internal.util.Preconditions.outOfBoundsCheckIndex(Preconditions.java:70)
+        at java.base/jdk.internal.util.Preconditions.checkIndex(Preconditions.java:248)
+        at java.base/java.util.Objects.checkIndex(Objects.java:372)
+        at java.base/java.util.ArrayList.get(ArrayList.java:459)
+        at java_programs.KTH.kth(KTH.java:5)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_programs.KTH.kth(KTH.java:22)
+        at java_testcases.junit.KTH_TEST.test_6(KTH_TEST.java:43)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  8,test_6(java_testcases.junit.KTH_TEST)
+%RUNTIME140</t>
+  </si>
+  <si>
+    <t>%TESTC  9 v2
+%TSTTREE1,java_testcases.junit.LCS_LENGTH_TEST,true,9,false,-1,java_testcases.junit.LCS_LENGTH_TEST,,
+%TSTTREE2,test_0(java_testcases.junit.LCS_LENGTH_TEST),false,1,false,-1,test_0(java_testcases.junit.LCS_LENGTH_TEST),,
+%TSTTREE3,test_1(java_testcases.junit.LCS_LENGTH_TEST),false,1,false,-1,test_1(java_testcases.junit.LCS_LENGTH_TEST),,
+%TSTTREE4,test_2(java_testcases.junit.LCS_LENGTH_TEST),false,1,false,-1,test_2(java_testcases.junit.LCS_LENGTH_TEST),,
+%TSTTREE5,test_3(java_testcases.junit.LCS_LENGTH_TEST),false,1,false,-1,test_3(java_testcases.junit.LCS_LENGTH_TEST),,
+%TSTTREE6,test_4(java_testcases.junit.LCS_LENGTH_TEST),false,1,false,-1,test_4(java_testcases.junit.LCS_LENGTH_TEST),,
+%TSTTREE7,test_5(java_testcases.junit.LCS_LENGTH_TEST),false,1,false,-1,test_5(java_testcases.junit.LCS_LENGTH_TEST),,
+%TSTTREE8,test_6(java_testcases.junit.LCS_LENGTH_TEST),false,1,false,-1,test_6(java_testcases.junit.LCS_LENGTH_TEST),,
+%TSTTREE9,test_7(java_testcases.junit.LCS_LENGTH_TEST),false,1,false,-1,test_7(java_testcases.junit.LCS_LENGTH_TEST),,
+%TSTTREE10,test_8(java_testcases.junit.LCS_LENGTH_TEST),false,1,false,-1,test_8(java_testcases.junit.LCS_LENGTH_TEST),,
+%TESTS  2,test_0(java_testcases.junit.LCS_LENGTH_TEST)
+%FAILED 2,test_0(java_testcases.junit.LCS_LENGTH_TEST)
+%TRACES 
+java.lang.AssertionError: expected:&lt;2&gt; but was:&lt;1&gt;
+        at org.junit.Assert.fail(Assert.java:89)
+        at org.junit.Assert.failNotEquals(Assert.java:835)
+        at org.junit.Assert.assertEquals(Assert.java:120)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LCS_LENGTH_TEST.test_0(LCS_LENGTH_TEST.java:8)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  2,test_0(java_testcases.junit.LCS_LENGTH_TEST)
+%TESTS  3,test_1(java_testcases.junit.LCS_LENGTH_TEST)
+%FAILED 3,test_1(java_testcases.junit.LCS_LENGTH_TEST)
+%TRACES 
+java.lang.AssertionError: expected:&lt;4&gt; but was:&lt;1&gt;
+        at org.junit.Assert.fail(Assert.java:89)
+        at org.junit.Assert.failNotEquals(Assert.java:835)
+        at org.junit.Assert.assertEquals(Assert.java:120)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LCS_LENGTH_TEST.test_1(LCS_LENGTH_TEST.java:14)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  3,test_1(java_testcases.junit.LCS_LENGTH_TEST)
+%TESTS  4,test_2(java_testcases.junit.LCS_LENGTH_TEST)
+%TESTE  4,test_2(java_testcases.junit.LCS_LENGTH_TEST)
+%TESTS  5,test_3(java_testcases.junit.LCS_LENGTH_TEST)
+%FAILED 5,test_3(java_testcases.junit.LCS_LENGTH_TEST)
+%TRACES 
+java.lang.AssertionError: expected:&lt;3&gt; but was:&lt;1&gt;
+        at org.junit.Assert.fail(Assert.java:89)
+        at org.junit.Assert.failNotEquals(Assert.java:835)
+        at org.junit.Assert.assertEquals(Assert.java:120)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LCS_LENGTH_TEST.test_3(LCS_LENGTH_TEST.java:26)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  5,test_3(java_testcases.junit.LCS_LENGTH_TEST)
+%TESTS  6,test_4(java_testcases.junit.LCS_LENGTH_TEST)
+%FAILED 6,test_4(java_testcases.junit.LCS_LENGTH_TEST)
+%TRACES 
+java.lang.AssertionError: expected:&lt;3&gt; but was:&lt;1&gt;
+        at org.junit.Assert.fail(Assert.java:89)
+        at org.junit.Assert.failNotEquals(Assert.java:835)
+        at org.junit.Assert.assertEquals(Assert.java:120)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LCS_LENGTH_TEST.test_4(LCS_LENGTH_TEST.java:32)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  6,test_4(java_testcases.junit.LCS_LENGTH_TEST)
+%TESTS  7,test_5(java_testcases.junit.LCS_LENGTH_TEST)
+%FAILED 7,test_5(java_testcases.junit.LCS_LENGTH_TEST)
+%TRACES 
+java.lang.AssertionError: expected:&lt;7&gt; but was:&lt;1&gt;
+        at org.junit.Assert.fail(Assert.java:89)
+        at org.junit.Assert.failNotEquals(Assert.java:835)
+        at org.junit.Assert.assertEquals(Assert.java:120)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LCS_LENGTH_TEST.test_5(LCS_LENGTH_TEST.java:38)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  7,test_5(java_testcases.junit.LCS_LENGTH_TEST)
+%TESTS  8,test_6(java_testcases.junit.LCS_LENGTH_TEST)
+%FAILED 8,test_6(java_testcases.junit.LCS_LENGTH_TEST)
+%TRACES 
+java.lang.AssertionError: expected:&lt;6&gt; but was:&lt;1&gt;
+        at org.junit.Assert.fail(Assert.java:89)
+        at org.junit.Assert.failNotEquals(Assert.java:835)
+        at org.junit.Assert.assertEquals(Assert.java:120)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LCS_LENGTH_TEST.test_6(LCS_LENGTH_TEST.java:44)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  8,test_6(java_testcases.junit.LCS_LENGTH_TEST)
+%TESTS  9,test_7(java_testcases.junit.LCS_LENGTH_TEST)
+%FAILED 9,test_7(java_testcases.junit.LCS_LENGTH_TEST)
+%TRACES 
+java.lang.AssertionError: expected:&lt;3&gt; but was:&lt;2&gt;
+        at org.junit.Assert.fail(Assert.java:89)
+        at org.junit.Assert.failNotEquals(Assert.java:835)
+        at org.junit.Assert.assertEquals(Assert.java:120)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LCS_LENGTH_TEST.test_7(LCS_LENGTH_TEST.java:50)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  9,test_7(java_testcases.junit.LCS_LENGTH_TEST)
+%TESTS  10,test_8(java_testcases.junit.LCS_LENGTH_TEST)
+%FAILED 10,test_8(java_testcases.junit.LCS_LENGTH_TEST)
+%TRACES 
+java.lang.AssertionError: expected:&lt;3&gt; but was:&lt;1&gt;
+        at org.junit.Assert.fail(Assert.java:89)
+        at org.junit.Assert.failNotEquals(Assert.java:835)
+        at org.junit.Assert.assertEquals(Assert.java:120)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LCS_LENGTH_TEST.test_8(LCS_LENGTH_TEST.java:56)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  10,test_8(java_testcases.junit.LCS_LENGTH_TEST)
+%RUNTIME110</t>
+  </si>
+  <si>
+    <t>%TESTC  10 v2
+%TSTTREE1,java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST,true,10,false,-1,java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST,,
+%TSTTREE2,test_0(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),false,1,false,-1,test_0(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),,
+%TSTTREE3,test_1(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),false,1,false,-1,test_1(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),,
+%TSTTREE4,test_2(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),false,1,false,-1,test_2(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),,
+%TSTTREE5,test_3(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),false,1,false,-1,test_3(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),,
+%TSTTREE6,test_4(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),false,1,false,-1,test_4(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),,
+%TSTTREE7,test_5(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),false,1,false,-1,test_5(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),,
+%TSTTREE8,test_6(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),false,1,false,-1,test_6(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),,
+%TSTTREE9,test_7(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),false,1,false,-1,test_7(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),,
+%TSTTREE10,test_8(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),false,1,false,-1,test_8(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),,
+%TSTTREE11,test_9(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),false,1,false,-1,test_9(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST),,
+%TESTS  2,test_0(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTE  2,test_0(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTS  3,test_1(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTE  3,test_1(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTS  4,test_2(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTE  4,test_2(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTS  5,test_3(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%FAILED 5,test_3(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%EXPECTS
+tsitest
+%EXPECTE
+%ACTUALS
+tiitest
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;t[s]itest&gt; but was:&lt;t[i]itest&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST.test_3(LONGEST_COMMON_SUBSEQUENCE_TEST.java:30)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  5,test_3(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTS  6,test_4(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTE  6,test_4(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTS  7,test_5(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%FAILED 7,test_5(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%EXPECTS
+bcba
+%EXPECTE
+%ACTUALS
+bbdab
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;b[cba]&gt; but was:&lt;b[bdab]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST.test_5(LONGEST_COMMON_SUBSEQUENCE_TEST.java:44)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  7,test_5(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTS  8,test_6(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%FAILED 8,test_6(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%EXPECTS
+TAAG
+%EXPECTE
+%ACTUALS
+TAAGC
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;TAAG[]&gt; but was:&lt;TAAG[C]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST.test_6(LONGEST_COMMON_SUBSEQUENCE_TEST.java:51)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  8,test_6(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTS  9,test_7(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%FAILED 9,test_7(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%EXPECTS
+BCBA
+%EXPECTE
+%ACTUALS
+BBDAB
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;B[CBA]&gt; but was:&lt;B[BDAB]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST.test_7(LONGEST_COMMON_SUBSEQUENCE_TEST.java:58)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  9,test_7(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTS  10,test_8(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTE  10,test_8(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTS  11,test_9(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%TESTE  11,test_9(java_testcases.junit.LONGEST_COMMON_SUBSEQUENCE_TEST)
+%RUNTIME458</t>
+  </si>
+  <si>
+    <t>%TESTC  13 v2
+%TSTTREE1,java_testcases.junit.MERGESORT_TEST,true,13,false,-1,java_testcases.junit.MERGESORT_TEST,,
+%TSTTREE2,test_10(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_10(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE3,test_11(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_11(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE4,test_12(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_12(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE5,test_0(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_0(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE6,test_1(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_1(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE7,test_2(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_2(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE8,test_3(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_3(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE9,test_4(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_4(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE10,test_5(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_5(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE11,test_6(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_6(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE12,test_7(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_7(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE13,test_8(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_8(java_testcases.junit.MERGESORT_TEST),,
+%TSTTREE14,test_9(java_testcases.junit.MERGESORT_TEST),false,1,false,-1,test_9(java_testcases.junit.MERGESORT_TEST),,
+%TESTS  2,test_10(java_testcases.junit.MERGESORT_TEST)
+%ERROR  2,test_10(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_10(MERGESORT_TEST.java:77)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  2,test_10(java_testcases.junit.MERGESORT_TEST)
+%TESTS  3,test_11(java_testcases.junit.MERGESORT_TEST)
+%ERROR  3,test_11(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_11(MERGESORT_TEST.java:84)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  3,test_11(java_testcases.junit.MERGESORT_TEST)
+%TESTS  4,test_12(java_testcases.junit.MERGESORT_TEST)
+%ERROR  4,test_12(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_12(MERGESORT_TEST.java:91)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  4,test_12(java_testcases.junit.MERGESORT_TEST)
+%TESTS  5,test_0(java_testcases.junit.MERGESORT_TEST)
+%ERROR  5,test_0(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_0(MERGESORT_TEST.java:7)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  5,test_0(java_testcases.junit.MERGESORT_TEST)
+%TESTS  6,test_1(java_testcases.junit.MERGESORT_TEST)
+%ERROR  6,test_1(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_1(MERGESORT_TEST.java:14)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  6,test_1(java_testcases.junit.MERGESORT_TEST)
+%TESTS  7,test_2(java_testcases.junit.MERGESORT_TEST)
+%ERROR  7,test_2(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_2(MERGESORT_TEST.java:21)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  7,test_2(java_testcases.junit.MERGESORT_TEST)
+%TESTS  8,test_3(java_testcases.junit.MERGESORT_TEST)
+%ERROR  8,test_3(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_3(MERGESORT_TEST.java:28)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  8,test_3(java_testcases.junit.MERGESORT_TEST)
+%TESTS  9,test_4(java_testcases.junit.MERGESORT_TEST)
+%ERROR  9,test_4(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_4(MERGESORT_TEST.java:35)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  9,test_4(java_testcases.junit.MERGESORT_TEST)
+%TESTS  10,test_5(java_testcases.junit.MERGESORT_TEST)
+%ERROR  10,test_5(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_5(MERGESORT_TEST.java:42)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  10,test_5(java_testcases.junit.MERGESORT_TEST)
+%TESTS  11,test_6(java_testcases.junit.MERGESORT_TEST)
+%ERROR  11,test_6(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_6(MERGESORT_TEST.java:49)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  11,test_6(java_testcases.junit.MERGESORT_TEST)
+%TESTS  12,test_7(java_testcases.junit.MERGESORT_TEST)
+%ERROR  12,test_7(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_7(MERGESORT_TEST.java:56)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  12,test_7(java_testcases.junit.MERGESORT_TEST)
+%TESTS  13,test_8(java_testcases.junit.MERGESORT_TEST)
+%ERROR  13,test_8(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_8(MERGESORT_TEST.java:63)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  13,test_8(java_testcases.junit.MERGESORT_TEST)
+%TESTS  14,test_9(java_testcases.junit.MERGESORT_TEST)
+%ERROR  14,test_9(java_testcases.junit.MERGESORT_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        The method merge(ArrayList&lt;Integer&gt;, ArrayList&lt;Integer&gt;) is undefined for the type MERGESORT
+        at java_programs.MERGESORT.mergesort(MERGESORT.java:18)
+        at java_testcases.junit.MERGESORT_TEST.test_9(MERGESORT_TEST.java:70)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  14,test_9(java_testcases.junit.MERGESORT_TEST)
+%RUNTIME355</t>
+  </si>
+  <si>
+    <t>%TESTC  3 v2
+%TSTTREE1,java_testcases.junit.MINIMUM_SPANNING_TREE_TEST,true,3,false,-1,java_testcases.junit.MINIMUM_SPANNING_TREE_TEST,,
+%TSTTREE2,test1(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST),false,1,false,-1,test1(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST),,
+%TSTTREE3,test2(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST),false,1,false,-1,test2(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST),,
+%TSTTREE4,test3(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST),false,1,false,-1,test3(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST),,
+%TESTS  2,test1(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST)
+%FAILED 2,test1(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST)
+%TRACES 
+java.lang.AssertionError: expected:&lt;true&gt; but was:&lt;false&gt;
+        at org.junit.Assert.fail(Assert.java:89)
+        at org.junit.Assert.failNotEquals(Assert.java:835)
+        at org.junit.Assert.assertEquals(Assert.java:120)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.MINIMUM_SPANNING_TREE_TEST.test1(MINIMUM_SPANNING_TREE_TEST.java:45)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  2,test1(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST)
+%TESTS  3,test2(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST)
+%FAILED 3,test2(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST)
+%TRACES 
+java.lang.AssertionError: expected:&lt;true&gt; but was:&lt;false&gt;
+        at org.junit.Assert.fail(Assert.java:89)
+        at org.junit.Assert.failNotEquals(Assert.java:835)
+        at org.junit.Assert.assertEquals(Assert.java:120)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.MINIMUM_SPANNING_TREE_TEST.test2(MINIMUM_SPANNING_TREE_TEST.java:82)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  3,test2(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST)
+%TESTS  4,test3(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST)
+%TESTE  4,test3(java_testcases.junit.MINIMUM_SPANNING_TREE_TEST)
+%RUNTIME68</t>
+  </si>
+  <si>
+    <t>%TESTC  5 v2
+%TSTTREE1,java_testcases.junit.NEXT_PALINDROME_TEST,true,5,false,-1,java_testcases.junit.NEXT_PALINDROME_TEST,,
+%TSTTREE2,test_0(java_testcases.junit.NEXT_PALINDROME_TEST),false,1,false,-1,test_0(java_testcases.junit.NEXT_PALINDROME_TEST),,
+%TSTTREE3,test_1(java_testcases.junit.NEXT_PALINDROME_TEST),false,1,false,-1,test_1(java_testcases.junit.NEXT_PALINDROME_TEST),,
+%TSTTREE4,test_2(java_testcases.junit.NEXT_PALINDROME_TEST),false,1,false,-1,test_2(java_testcases.junit.NEXT_PALINDROME_TEST),,
+%TSTTREE5,test_3(java_testcases.junit.NEXT_PALINDROME_TEST),false,1,false,-1,test_3(java_testcases.junit.NEXT_PALINDROME_TEST),,
+%TSTTREE6,test_4(java_testcases.junit.NEXT_PALINDROME_TEST),false,1,false,-1,test_4(java_testcases.junit.NEXT_PALINDROME_TEST),,
+%TESTS  2,test_0(java_testcases.junit.NEXT_PALINDROME_TEST)
+%TESTE  2,test_0(java_testcases.junit.NEXT_PALINDROME_TEST)
+%TESTS  3,test_1(java_testcases.junit.NEXT_PALINDROME_TEST)
+%TESTE  3,test_1(java_testcases.junit.NEXT_PALINDROME_TEST)
+%TESTS  4,test_2(java_testcases.junit.NEXT_PALINDROME_TEST)
+%TESTE  4,test_2(java_testcases.junit.NEXT_PALINDROME_TEST)
+%TESTS  5,test_3(java_testcases.junit.NEXT_PALINDROME_TEST)
+%TESTE  5,test_3(java_testcases.junit.NEXT_PALINDROME_TEST)
+%TESTS  6,test_4(java_testcases.junit.NEXT_PALINDROME_TEST)
+%FAILED 6,test_4(java_testcases.junit.NEXT_PALINDROME_TEST)
+%EXPECTS</t>
+  </si>
+  <si>
+    <t>%TESTC  5 v2
+%TSTTREE1,java_testcases.junit.POWERSET_TEST,true,5,false,-1,java_testcases.junit.POWERSET_TEST,,
+%TSTTREE2,test_0(java_testcases.junit.POWERSET_TEST),false,1,false,-1,test_0(java_testcases.junit.POWERSET_TEST),,
+%TSTTREE3,test_1(java_testcases.junit.POWERSET_TEST),false,1,false,-1,test_1(java_testcases.junit.POWERSET_TEST),,
+%TSTTREE4,test_2(java_testcases.junit.POWERSET_TEST),false,1,false,-1,test_2(java_testcases.junit.POWERSET_TEST),,
+%TSTTREE5,test_3(java_testcases.junit.POWERSET_TEST),false,1,false,-1,test_3(java_testcases.junit.POWERSET_TEST),,
+%TSTTREE6,test_4(java_testcases.junit.POWERSET_TEST),false,1,false,-1,test_4(java_testcases.junit.POWERSET_TEST),,
+%TESTS  2,test_0(java_testcases.junit.POWERSET_TEST)
+%FAILED 2,test_0(java_testcases.junit.POWERSET_TEST)
+%EXPECTS
+[[],[c],[b],[b,c],[a],[a,c],[a,b],[a,b,c]]
+%EXPECTE
+%ACTUALS
+[[a,b,c],[b,c],[a,c],[c],[a,b],[b],[a],[]]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[],[c],[b],[b,c],[a],[a,c],[a,b],[a,b,c]]]&gt; but was:&lt;[[[a,b,c],[b,c],[a,c],[c],[a,b],[b],[a],[]]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.POWERSET_TEST.test_0(POWERSET_TEST.java:9)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  2,test_0(java_testcases.junit.POWERSET_TEST)
+%TESTS  3,test_1(java_testcases.junit.POWERSET_TEST)
+%FAILED 3,test_1(java_testcases.junit.POWERSET_TEST)
+%EXPECTS
+[[],[b],[a],[a,b]]
+%EXPECTE
+%ACTUALS
+[[a,b],[b],[a],[]]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[],[b],[a],[a,b]]]&gt; but was:&lt;[[[a,b],[b],[a],[]]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.POWERSET_TEST.test_1(POWERSET_TEST.java:16)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  3,test_1(java_testcases.junit.POWERSET_TEST)
+%TESTS  4,test_2(java_testcases.junit.POWERSET_TEST)
+%FAILED 4,test_2(java_testcases.junit.POWERSET_TEST)
+%EXPECTS
+[[],[a]]
+%EXPECTE
+%ACTUALS
+[[a],[]]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[],[a]]]&gt; but was:&lt;[[[a],[]]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.POWERSET_TEST.test_2(POWERSET_TEST.java:23)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  4,test_2(java_testcases.junit.POWERSET_TEST)
+%TESTS  5,test_3(java_testcases.junit.POWERSET_TEST)
+%TESTE  5,test_3(java_testcases.junit.POWERSET_TEST)
+%TESTS  6,test_4(java_testcases.junit.POWERSET_TEST)
+%FAILED 6,test_4(java_testcases.junit.POWERSET_TEST)
+%EXPECTS
+[[],[m],[z],[z,m],[df],[df,m],[df,z],[df,z,m],[x],[x,m],[x,z],[x,z,m],[x,df],[x,df,m],[x,df,z],[x,df,z,m]]
+%EXPECTE
+%ACTUALS
+[[x,df,z,m],[df,z,m],[x,z,m],[z,m],[x,df,m],[df,m],[x,m],[m],[x,df,z],[df,z],[x,z],[z],[x,df],[df],[x],[]]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[],[m],[z],[z,m],[df],[df,m],[df,z],[df,z,m],[x],[x,m],[x,z],[x,z,m],[x,df],[x,df,m],[x,df,z],[x,df,z,m]]]&gt; but was:&lt;[[[x,df,z,m],[df,z,m],[x,z,m],[z,m],[x,df,m],[df,m],[x,m],[m],[x,df,z],[df,z],[x,z],[z],[x,df],[df],[x],[]]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.POWERSET_TEST.test_4(POWERSET_TEST.java:37)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  6,test_4(java_testcases.junit.POWERSET_TEST)
+%RUNTIME351</t>
+  </si>
+  <si>
+    <t>%TESTC  3 v2
+%TSTTREE1,java_testcases.junit.SHORTEST_PATHS_TEST,true,3,false,-1,java_testcases.junit.SHORTEST_PATHS_TEST,,
+%TSTTREE2,test1(java_testcases.junit.SHORTEST_PATHS_TEST),false,1,false,-1,test1(java_testcases.junit.SHORTEST_PATHS_TEST),,
+%TSTTREE3,test2(java_testcases.junit.SHORTEST_PATHS_TEST),false,1,false,-1,test2(java_testcases.junit.SHORTEST_PATHS_TEST),,
+%TSTTREE4,test3(java_testcases.junit.SHORTEST_PATHS_TEST),false,1,false,-1,test3(java_testcases.junit.SHORTEST_PATHS_TEST),,
+%TESTS  2,test1(java_testcases.junit.SHORTEST_PATHS_TEST)
+%ERROR  2,test1(java_testcases.junit.SHORTEST_PATHS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        SHORTEST_PATHS cannot be resolved
+        at java_testcases.junit.SHORTEST_PATHS_TEST.test1(SHORTEST_PATHS_TEST.java:32)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.BlockJUnit4ClassRunner$1.evaluate(BlockJUnit4ClassRunner.java:100)
+        at org.junit.runners.ParentRunner.runLeaf(ParentRunner.java:366)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:103)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:63)
+        at org.junit.runners.ParentRunner$4.run(ParentRunner.java:331)
+        at org.junit.runners.ParentRunner$1.schedule(ParentRunner.java:79)
+        at org.junit.runners.ParentRunner.runChildren(ParentRunner.java:329)
+        at org.junit.runners.ParentRunner.access$100(ParentRunner.java:66)
+        at org.junit.runners.ParentRunner$2.evaluate(ParentRunner.java:293)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.ParentRunner.run(ParentRunner.java:413)
+        at org.eclipse.jdt.internal.junit4.runner.JUnit4TestReference.run(JUnit4TestReference.java:93)
+        at org.eclipse.jdt.internal.junit.runner.TestExecution.run(TestExecution.java:40)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:530)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:758)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.run(RemoteTestRunner.java:453)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.main(RemoteTestRunner.java:211)
+%TRACEE 
+%TESTE  2,test1(java_testcases.junit.SHORTEST_PATHS_TEST)
+%TESTS  3,test2(java_testcases.junit.SHORTEST_PATHS_TEST)
+%ERROR  3,test2(java_testcases.junit.SHORTEST_PATHS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        SHORTEST_PATHS cannot be resolved
+        at java_testcases.junit.SHORTEST_PATHS_TEST.test2(SHORTEST_PATHS_TEST.java:53)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.BlockJUnit4ClassRunner$1.evaluate(BlockJUnit4ClassRunner.java:100)
+        at org.junit.runners.ParentRunner.runLeaf(ParentRunner.java:366)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:103)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:63)
+        at org.junit.runners.ParentRunner$4.run(ParentRunner.java:331)
+        at org.junit.runners.ParentRunner$1.schedule(ParentRunner.java:79)
+        at org.junit.runners.ParentRunner.runChildren(ParentRunner.java:329)
+        at org.junit.runners.ParentRunner.access$100(ParentRunner.java:66)
+        at org.junit.runners.ParentRunner$2.evaluate(ParentRunner.java:293)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.ParentRunner.run(ParentRunner.java:413)
+        at org.eclipse.jdt.internal.junit4.runner.JUnit4TestReference.run(JUnit4TestReference.java:93)
+        at org.eclipse.jdt.internal.junit.runner.TestExecution.run(TestExecution.java:40)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:530)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:758)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.run(RemoteTestRunner.java:453)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.main(RemoteTestRunner.java:211)
+%TRACEE 
+%TESTE  3,test2(java_testcases.junit.SHORTEST_PATHS_TEST)
+%TESTS  4,test3(java_testcases.junit.SHORTEST_PATHS_TEST)
+%ERROR  4,test3(java_testcases.junit.SHORTEST_PATHS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        SHORTEST_PATHS cannot be resolved
+        at java_testcases.junit.SHORTEST_PATHS_TEST.test3(SHORTEST_PATHS_TEST.java:75)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.BlockJUnit4ClassRunner$1.evaluate(BlockJUnit4ClassRunner.java:100)
+        at org.junit.runners.ParentRunner.runLeaf(ParentRunner.java:366)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:103)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:63)
+        at org.junit.runners.ParentRunner$4.run(ParentRunner.java:331)
+        at org.junit.runners.ParentRunner$1.schedule(ParentRunner.java:79)
+        at org.junit.runners.ParentRunner.runChildren(ParentRunner.java:329)
+        at org.junit.runners.ParentRunner.access$100(ParentRunner.java:66)
+        at org.junit.runners.ParentRunner$2.evaluate(ParentRunner.java:293)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.ParentRunner.run(ParentRunner.java:413)
+        at org.eclipse.jdt.internal.junit4.runner.JUnit4TestReference.run(JUnit4TestReference.java:93)
+        at org.eclipse.jdt.internal.junit.runner.TestExecution.run(TestExecution.java:40)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:530)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:758)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.run(RemoteTestRunner.java:453)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.main(RemoteTestRunner.java:211)
+%TRACEE 
+%TESTE  4,test3(java_testcases.junit.SHORTEST_PATHS_TEST)
+%RUNTIME91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%TESTC  4 v2
+%TSTTREE1,java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST,true,4,false,-1,java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST,,
+%TSTTREE2,test4s(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST),false,1,false,-1,test4s(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST),,
+%TSTTREE3,test1(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST),false,1,false,-1,test1(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST),,
+%TSTTREE4,test2(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST),false,1,false,-1,test2(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST),,
+%TSTTREE5,test3(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST),false,1,false,-1,test3(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST),,
+%TESTS  2,test4s(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%ERROR  2,test4s(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problems: 
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        edge cannot be resolved to a variable
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        update_length cannot be resolved to a variable
+        at java_programs.SHORTEST_PATH_LENGTHS.shortest_path_lengths(SHORTEST_PATHS.java:25)
+        at java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST.test4s(SHORTEST_PATH_LENGTHS_TEST.java:81)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.BlockJUnit4ClassRunner$1.evaluate(BlockJUnit4ClassRunner.java:100)
+        at org.junit.runners.ParentRunner.runLeaf(ParentRunner.java:366)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:103)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:63)
+        at org.junit.runners.ParentRunner$4.run(ParentRunner.java:331)
+        at org.junit.runners.ParentRunner$1.schedule(ParentRunner.java:79)
+        at org.junit.runners.ParentRunner.runChildren(ParentRunner.java:329)
+        at org.junit.runners.ParentRunner.access$100(ParentRunner.java:66)
+        at org.junit.runners.ParentRunner$2.evaluate(ParentRunner.java:293)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.ParentRunner.run(ParentRunner.java:413)
+        at org.eclipse.jdt.internal.junit4.runner.JUnit4TestReference.run(JUnit4TestReference.java:93)
+        at org.eclipse.jdt.internal.junit.runner.TestExecution.run(TestExecution.java:40)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:530)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:758)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.run(RemoteTestRunner.java:453)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.main(RemoteTestRunner.java:211)
+%TRACEE 
+%TESTE  2,test4s(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%TESTS  3,test1(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%ERROR  3,test1(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problems: 
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        edge cannot be resolved to a variable
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        update_length cannot be resolved to a variable
+        at java_programs.SHORTEST_PATH_LENGTHS.shortest_path_lengths(SHORTEST_PATHS.java:25)
+        at java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST.test1(SHORTEST_PATH_LENGTHS_TEST.java:27)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.BlockJUnit4ClassRunner$1.evaluate(BlockJUnit4ClassRunner.java:100)
+        at org.junit.runners.ParentRunner.runLeaf(ParentRunner.java:366)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:103)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:63)
+        at org.junit.runners.ParentRunner$4.run(ParentRunner.java:331)
+        at org.junit.runners.ParentRunner$1.schedule(ParentRunner.java:79)
+        at org.junit.runners.ParentRunner.runChildren(ParentRunner.java:329)
+        at org.junit.runners.ParentRunner.access$100(ParentRunner.java:66)
+        at org.junit.runners.ParentRunner$2.evaluate(ParentRunner.java:293)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.ParentRunner.run(ParentRunner.java:413)
+        at org.eclipse.jdt.internal.junit4.runner.JUnit4TestReference.run(JUnit4TestReference.java:93)
+        at org.eclipse.jdt.internal.junit.runner.TestExecution.run(TestExecution.java:40)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:530)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:758)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.run(RemoteTestRunner.java:453)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.main(RemoteTestRunner.java:211)
+%TRACEE 
+%TESTE  3,test1(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%TESTS  4,test2(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%ERROR  4,test2(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problems: 
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        edge cannot be resolved to a variable
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        update_length cannot be resolved to a variable
+        at java_programs.SHORTEST_PATH_LENGTHS.shortest_path_lengths(SHORTEST_PATHS.java:25)
+        at java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST.test2(SHORTEST_PATH_LENGTHS_TEST.java:46)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.BlockJUnit4ClassRunner$1.evaluate(BlockJUnit4ClassRunner.java:100)
+        at org.junit.runners.ParentRunner.runLeaf(ParentRunner.java:366)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:103)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:63)
+        at org.junit.runners.ParentRunner$4.run(ParentRunner.java:331)
+        at org.junit.runners.ParentRunner$1.schedule(ParentRunner.java:79)
+        at org.junit.runners.ParentRunner.runChildren(ParentRunner.java:329)
+        at org.junit.runners.ParentRunner.access$100(ParentRunner.java:66)
+        at org.junit.runners.ParentRunner$2.evaluate(ParentRunner.java:293)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.ParentRunner.run(ParentRunner.java:413)
+        at org.eclipse.jdt.internal.junit4.runner.JUnit4TestReference.run(JUnit4TestReference.java:93)
+        at org.eclipse.jdt.internal.junit.runner.TestExecution.run(TestExecution.java:40)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:530)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:758)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.run(RemoteTestRunner.java:453)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.main(RemoteTestRunner.java:211)
+%TRACEE 
+%TESTE  4,test2(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%TESTS  5,test3(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%ERROR  5,test3(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problems: 
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        edge cannot be resolved to a variable
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        weight_by_node cannot be resolved
+        edge cannot be resolved
+        update_length cannot be resolved to a variable
+        at java_programs.SHORTEST_PATH_LENGTHS.shortest_path_lengths(SHORTEST_PATHS.java:25)
+        at java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST.test3(SHORTEST_PATH_LENGTHS_TEST.java:63)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.BlockJUnit4ClassRunner$1.evaluate(BlockJUnit4ClassRunner.java:100)
+        at org.junit.runners.ParentRunner.runLeaf(ParentRunner.java:366)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:103)
+        at org.junit.runners.BlockJUnit4ClassRunner.runChild(BlockJUnit4ClassRunner.java:63)
+        at org.junit.runners.ParentRunner$4.run(ParentRunner.java:331)
+        at org.junit.runners.ParentRunner$1.schedule(ParentRunner.java:79)
+        at org.junit.runners.ParentRunner.runChildren(ParentRunner.java:329)
+        at org.junit.runners.ParentRunner.access$100(ParentRunner.java:66)
+        at org.junit.runners.ParentRunner$2.evaluate(ParentRunner.java:293)
+        at org.junit.runners.ParentRunner$3.evaluate(ParentRunner.java:306)
+        at org.junit.runners.ParentRunner.run(ParentRunner.java:413)
+        at org.eclipse.jdt.internal.junit4.runner.JUnit4TestReference.run(JUnit4TestReference.java:93)
+        at org.eclipse.jdt.internal.junit.runner.TestExecution.run(TestExecution.java:40)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:530)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.runTests(RemoteTestRunner.java:758)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.run(RemoteTestRunner.java:453)
+        at org.eclipse.jdt.internal.junit.runner.RemoteTestRunner.main(RemoteTestRunner.java:211)
+%TRACEE 
+%TESTE  5,test3(java_testcases.junit.SHORTEST_PATH_LENGTHS_TEST)
+%RUNTIME79
+</t>
+  </si>
+  <si>
+    <t>%TESTC  4 v2
+%TSTTREE1,java_testcases.junit.SHUNTING_YARD_TEST,true,4,false,-1,java_testcases.junit.SHUNTING_YARD_TEST,,
+%TSTTREE2,test_0(java_testcases.junit.SHUNTING_YARD_TEST),false,1,false,-1,test_0(java_testcases.junit.SHUNTING_YARD_TEST),,
+%TSTTREE3,test_1(java_testcases.junit.SHUNTING_YARD_TEST),false,1,false,-1,test_1(java_testcases.junit.SHUNTING_YARD_TEST),,
+%TSTTREE4,test_2(java_testcases.junit.SHUNTING_YARD_TEST),false,1,false,-1,test_2(java_testcases.junit.SHUNTING_YARD_TEST),,
+%TSTTREE5,test_3(java_testcases.junit.SHUNTING_YARD_TEST),false,1,false,-1,test_3(java_testcases.junit.SHUNTING_YARD_TEST),,
+%TESTS  2,test_0(java_testcases.junit.SHUNTING_YARD_TEST)
+%ERROR  2,test_0(java_testcases.junit.SHUNTING_YARD_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        This method must return a result of type List
+        at java_programs.SHUNTING_YARD.shunting_yard(SHUNTING_YARD.java:6)
+        at java_testcases.junit.SHUNTING_YARD_TEST.test_0(SHUNTING_YARD_TEST.java:7)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  2,test_0(java_testcases.junit.SHUNTING_YARD_TEST)
+%TESTS  3,test_1(java_testcases.junit.SHUNTING_YARD_TEST)
+%ERROR  3,test_1(java_testcases.junit.SHUNTING_YARD_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        This method must return a result of type List
+        at java_programs.SHUNTING_YARD.shunting_yard(SHUNTING_YARD.java:6)
+        at java_testcases.junit.SHUNTING_YARD_TEST.test_1(SHUNTING_YARD_TEST.java:14)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  3,test_1(java_testcases.junit.SHUNTING_YARD_TEST)
+%TESTS  4,test_2(java_testcases.junit.SHUNTING_YARD_TEST)
+%ERROR  4,test_2(java_testcases.junit.SHUNTING_YARD_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        This method must return a result of type List
+        at java_programs.SHUNTING_YARD.shunting_yard(SHUNTING_YARD.java:6)
+        at java_testcases.junit.SHUNTING_YARD_TEST.test_2(SHUNTING_YARD_TEST.java:21)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  4,test_2(java_testcases.junit.SHUNTING_YARD_TEST)
+%TESTS  5,test_3(java_testcases.junit.SHUNTING_YARD_TEST)
+%ERROR  5,test_3(java_testcases.junit.SHUNTING_YARD_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        This method must return a result of type List
+        at java_programs.SHUNTING_YARD.shunting_yard(SHUNTING_YARD.java:6)
+        at java_testcases.junit.SHUNTING_YARD_TEST.test_3(SHUNTING_YARD_TEST.java:28)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  5,test_3(java_testcases.junit.SHUNTING_YARD_TEST)
+%RUNTIME138</t>
+  </si>
+  <si>
+    <t>%TESTC  6 v2
+%TSTTREE1,java_testcases.junit.SIEVE_TEST,true,6,false,-1,java_testcases.junit.SIEVE_TEST,,
+%TSTTREE2,test_0(java_testcases.junit.SIEVE_TEST),false,1,false,-1,test_0(java_testcases.junit.SIEVE_TEST),,
+%TSTTREE3,test_1(java_testcases.junit.SIEVE_TEST),false,1,false,-1,test_1(java_testcases.junit.SIEVE_TEST),,
+%TSTTREE4,test_2(java_testcases.junit.SIEVE_TEST),false,1,false,-1,test_2(java_testcases.junit.SIEVE_TEST),,
+%TSTTREE5,test_3(java_testcases.junit.SIEVE_TEST),false,1,false,-1,test_3(java_testcases.junit.SIEVE_TEST),,
+%TSTTREE6,test_4(java_testcases.junit.SIEVE_TEST),false,1,false,-1,test_4(java_testcases.junit.SIEVE_TEST),,
+%TSTTREE7,test_5(java_testcases.junit.SIEVE_TEST),false,1,false,-1,test_5(java_testcases.junit.SIEVE_TEST),,
+%TESTS  2,test_0(java_testcases.junit.SIEVE_TEST)
+%ERROR  2,test_0(java_testcases.junit.SIEVE_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Local variable n defined in an enclosing scope must be final or effectively final
+        at java_programs.SIEVE.sieve(SIEVE.java:24)
+        at java_testcases.junit.SIEVE_TEST.test_0(SIEVE_TEST.java:7)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  2,test_0(java_testcases.junit.SIEVE_TEST)
+%TESTS  3,test_1(java_testcases.junit.SIEVE_TEST)
+%ERROR  3,test_1(java_testcases.junit.SIEVE_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Local variable n defined in an enclosing scope must be final or effectively final
+        at java_programs.SIEVE.sieve(SIEVE.java:24)
+        at java_testcases.junit.SIEVE_TEST.test_1(SIEVE_TEST.java:14)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  3,test_1(java_testcases.junit.SIEVE_TEST)
+%TESTS  4,test_2(java_testcases.junit.SIEVE_TEST)
+%ERROR  4,test_2(java_testcases.junit.SIEVE_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Local variable n defined in an enclosing scope must be final or effectively final
+        at java_programs.SIEVE.sieve(SIEVE.java:24)
+        at java_testcases.junit.SIEVE_TEST.test_2(SIEVE_TEST.java:21)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  4,test_2(java_testcases.junit.SIEVE_TEST)
+%TESTS  5,test_3(java_testcases.junit.SIEVE_TEST)
+%ERROR  5,test_3(java_testcases.junit.SIEVE_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Local variable n defined in an enclosing scope must be final or effectively final
+        at java_programs.SIEVE.sieve(SIEVE.java:24)
+        at java_testcases.junit.SIEVE_TEST.test_3(SIEVE_TEST.java:28)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  5,test_3(java_testcases.junit.SIEVE_TEST)
+%TESTS  6,test_4(java_testcases.junit.SIEVE_TEST)
+%ERROR  6,test_4(java_testcases.junit.SIEVE_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Local variable n defined in an enclosing scope must be final or effectively final
+        at java_programs.SIEVE.sieve(SIEVE.java:24)
+        at java_testcases.junit.SIEVE_TEST.test_4(SIEVE_TEST.java:35)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  6,test_4(java_testcases.junit.SIEVE_TEST)
+%TESTS  7,test_5(java_testcases.junit.SIEVE_TEST)
+%ERROR  7,test_5(java_testcases.junit.SIEVE_TEST)
+%TRACES 
+java.lang.Error: Unresolved compilation problem: 
+        Local variable n defined in an enclosing scope must be final or effectively final
+        at java_programs.SIEVE.sieve(SIEVE.java:24)
+        at java_testcases.junit.SIEVE_TEST.test_5(SIEVE_TEST.java:42)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  7,test_5(java_testcases.junit.SIEVE_TEST)
+%RUNTIME126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%TESTC  12 v2
+%TSTTREE1,java_testcases.junit.SUBSEQUENCES_TEST,true,12,false,-1,java_testcases.junit.SUBSEQUENCES_TEST,,
+%TSTTREE2,test_10(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_10(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TSTTREE3,test_11(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_11(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TSTTREE4,test_0(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_0(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TSTTREE5,test_1(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_1(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TSTTREE6,test_2(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_2(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TSTTREE7,test_3(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_3(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TSTTREE8,test_4(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_4(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TSTTREE9,test_5(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_5(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TSTTREE10,test_6(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_6(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TSTTREE11,test_7(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_7(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TSTTREE12,test_8(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_8(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TSTTREE13,test_9(java_testcases.junit.SUBSEQUENCES_TEST),false,1,false,-1,test_9(java_testcases.junit.SUBSEQUENCES_TEST),,
+%TESTS  2,test_10(java_testcases.junit.SUBSEQUENCES_TEST)
+%FAILED 2,test_10(java_testcases.junit.SUBSEQUENCES_TEST)
+%EXPECTS
+[[]]
+%EXPECTE
+%ACTUALS
+[]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[]]]&gt; but was:&lt;[[]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.SUBSEQUENCES_TEST.test_10(SUBSEQUENCES_TEST.java:79)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  2,test_10(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTS  3,test_11(java_testcases.junit.SUBSEQUENCES_TEST)
+%FAILED 3,test_11(java_testcases.junit.SUBSEQUENCES_TEST)
+%EXPECTS
+[[]]
+%EXPECTE
+%ACTUALS
+[]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[]]]&gt; but was:&lt;[[]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.SUBSEQUENCES_TEST.test_11(SUBSEQUENCES_TEST.java:86)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  3,test_11(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTS  4,test_0(java_testcases.junit.SUBSEQUENCES_TEST)
+%FAILED 4,test_0(java_testcases.junit.SUBSEQUENCES_TEST)
+%EXPECTS
+[[1,2,3],[1,2,4],[1,3,4],[2,3,4]]
+%EXPECTE
+%ACTUALS
+[]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[1,2,3],[1,2,4],[1,3,4],[2,3,4]]]&gt; but was:&lt;[[]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.SUBSEQUENCES_TEST.test_0(SUBSEQUENCES_TEST.java:9)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  4,test_0(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTS  5,test_1(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTE  5,test_1(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTS  6,test_2(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTE  6,test_2(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTS  7,test_3(java_testcases.junit.SUBSEQUENCES_TEST)
+%FAILED 7,test_3(java_testcases.junit.SUBSEQUENCES_TEST)
+%EXPECTS
+[[4,5,6,7],[4,5,6,8],[4,5,6,9],[4,5,7,8],[4,5,7,9],[4,5,8,9],[4,6,7,8],[4,6,7,9],[4,6,8,9],[4,7,8,9],[5,6,7,8],[5,6,7,9],[5,6,8,9],[5,7,8,9],[6,7,8,9]]
+%EXPECTE
+%ACTUALS
+[]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[4,5,6,7],[4,5,6,8],[4,5,6,9],[4,5,7,8],[4,5,7,9],[4,5,8,9],[4,6,7,8],[4,6,7,9],[4,6,8,9],[4,7,8,9],[5,6,7,8],[5,6,7,9],[5,6,8,9],[5,7,8,9],[6,7,8,9]]]&gt; but was:&lt;[[]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.SUBSEQUENCES_TEST.test_3(SUBSEQUENCES_TEST.java:30)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  7,test_3(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTS  8,test_4(java_testcases.junit.SUBSEQUENCES_TEST)
+%FAILED 8,test_4(java_testcases.junit.SUBSEQUENCES_TEST)
+%EXPECTS
+[[4,5,6,7,8,9]]
+%EXPECTE
+%ACTUALS
+[]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[4,5,6,7,8,9]]]&gt; but was:&lt;[[]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.SUBSEQUENCES_TEST.test_4(SUBSEQUENCES_TEST.java:37)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  8,test_4(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTS  9,test_5(java_testcases.junit.SUBSEQUENCES_TEST)
+%FAILED 9,test_5(java_testcases.junit.SUBSEQUENCES_TEST)
+%EXPECTS
+[[1,2],[1,3],[1,4],[1,5],[1,6],[1,7],[1,8],[1,9],[2,3],[2,4],[2,5],[2,6],[2,7],[2,8],[2,9],[3,4],[3,5],[3,6],[3,7],[3,8],[3,9],[4,5],[4,6],[4,7],[4,8],[4,9],[5,6],[5,7],[5,8],[5,9],[6,7],[6,8],[6,9],[7,8],[7,9],[8,9]]
+%EXPECTE
+%ACTUALS
+[]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[1,2],[1,3],[1,4],[1,5],[1,6],[1,7],[1,8],[1,9],[2,3],[2,4],[2,5],[2,6],[2,7],[2,8],[2,9],[3,4],[3,5],[3,6],[3,7],[3,8],[3,9],[4,5],[4,6],[4,7],[4,8],[4,9],[5,6],[5,7],[5,8],[5,9],[6,7],[6,8],[6,9],[7,8],[7,9],[8,9]]]&gt; but was:&lt;[[]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.SUBSEQUENCES_TEST.test_5(SUBSEQUENCES_TEST.java:44)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  9,test_5(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTS  10,test_6(java_testcases.junit.SUBSEQUENCES_TEST)
+%FAILED 10,test_6(java_testcases.junit.SUBSEQUENCES_TEST)
+%EXPECTS
+[[1,2,3,4,5,6],[1,2,3,4,5,7],[1,2,3,4,5,8],[1,2,3,4,5,9],[1,2,3,4,6,7],[1,2,3,4,6,8],[1,2,3,4,6,9],[1,2,3,4,7,8],[1,2,3,4,7,9],[1,2,3,4,8,9],[1,2,3,5,6,7],[1,2,3,5,6,8],[1,2,3,5,6,9],[1,2,3,5,7,8],[1,2,3,5,7,9],[1,2,3,5,8,9],[1,2,3,6,7,8],[1,2,3,6,7,9],[1,2,3,6,8,9],[1,2,3,7,8,9],[1,2,4,5,6,7],[1,2,4,5,6,8],[1,2,4,5,6,9],[1,2,4,5,7,8],[1,2,4,5,7,9],[1,2,4,5,8,9],[1,2,4,6,7,8],[1,2,4,6,7,9],[1,2,4,6,8,9],[1,2,4,7,8,9],[1,2,5,6,7,8],[1,2,5,6,7,9],[1,2,5,6,8,9],[1,2,5,7,8,9],[1,2,6,7,8,9],[1,3,4,5,6,7],[1,3,4,5,6,8],[1,3,4,5,6,9],[1,3,4,5,7,8],[1,3,4,5,7,9],[1,3,4,5,8,9],[1,3,4,6,7,8],[1,3,4,6,7,9],[1,3,4,6,8,9],[1,3,4,7,8,9],[1,3,5,6,7,8],[1,3,5,6,7,9],[1,3,5,6,8,9],[1,3,5,7,8,9],[1,3,6,7,8,9],[1,4,5,6,7,8],[1,4,5,6,7,9],[1,4,5,6,8,9],[1,4,5,7,8,9],[1,4,6,7,8,9],[1,5,6,7,8,9],[2,3,4,5,6,7],[2,3,4,5,6,8],[2,3,4,5,6,9],[2,3,4,5,7,8],[2,3,4,5,7,9],[2,3,4,5,8,9],[2,3,4,6,7,8],[2,3,4,6,7,9],[2,3,4,6,8,9],[2,3,4,7,8,9],[2,3,5,6,7,8],[2,3,5,6,7,9],[2,3,5,6,8,9],[2,3,5,7,8,9],[2,3,6,7,8,9],[2,4,5,6,7,8],[2,4,5,6,7,9],[2,4,5,6,8,9],[2,4,5,7,8,9],[2,4,6,7,8,9],[2,5,6,7,8,9],[3,4,5,6,7,8],[3,4,5,6,7,9],[3,4,5,6,8,9],[3,4,5,7,8,9],[3,4,6,7,8,9],[3,5,6,7,8,9],[4,5,6,7,8,9]]
+%EXPECTE
+%ACTUALS
+[]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[1,2,3,4,5,6],[1,2,3,4,5,7],[1,2,3,4,5,8],[1,2,3,4,5,9],[1,2,3,4,6,7],[1,2,3,4,6,8],[1,2,3,4,6,9],[1,2,3,4,7,8],[1,2,3,4,7,9],[1,2,3,4,8,9],[1,2,3,5,6,7],[1,2,3,5,6,8],[1,2,3,5,6,9],[1,2,3,5,7,8],[1,2,3,5,7,9],[1,2,3,5,8,9],[1,2,3,6,7,8],[1,2,3,6,7,9],[1,2,3,6,8,9],[1,2,3,7,8,9],[1,2,4,5,6,7],[1,2,4,5,6,8],[1,2,4,5,6,9],[1,2,4,5,7,8],[1,2,4,5,7,9],[1,2,4,5,8,9],[1,2,4,6,7,8],[1,2,4,6,7,9],[1,2,4,6,8,9],[1,2,4,7,8,9],[1,2,5,6,7,8],[1,2,5,6,7,9],[1,2,5,6,8,9],[1,2,5,7,8,9],[1,2,6,7,8,9],[1,3,4,5,6,7],[1,3,4,5,6,8],[1,3,4,5,6,9],[1,3,4,5,7,8],[1,3,4,5,7,9],[1,3,4,5,8,9],[1,3,4,6,7,8],[1,3,4,6,7,9],[1,3,4,6,8,9],[1,3,4,7,8,9],[1,3,5,6,7,8],[1,3,5,6,7,9],[1,3,5,6,8,9],[1,3,5,7,8,9],[1,3,6,7,8,9],[1,4,5,6,7,8],[1,4,5,6,7,9],[1,4,5,6,8,9],[1,4,5,7,8,9],[1,4,6,7,8,9],[1,5,6,7,8,9],[2,3,4,5,6,7],[2,3,4,5,6,8],[2,3,4,5,6,9],[2,3,4,5,7,8],[2,3,4,5,7,9],[2,3,4,5,8,9],[2,3,4,6,7,8],[2,3,4,6,7,9],[2,3,4,6,8,9],[2,3,4,7,8,9],[2,3,5,6,7,8],[2,3,5,6,7,9],[2,3,5,6,8,9],[2,3,5,7,8,9],[2,3,6,7,8,9],[2,4,5,6,7,8],[2,4,5,6,7,9],[2,4,5,6,8,9],[2,4,5,7,8,9],[2,4,6,7,8,9],[2,5,6,7,8,9],[3,4,5,6,7,8],[3,4,5,6,7,9],[3,4,5,6,8,9],[3,4,5,7,8,9],[3,4,6,7,8,9],[3,5,6,7,8,9],[4,5,6,7,8,9]]]&gt; but was:&lt;[[]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.SUBSEQUENCES_TEST.test_6(SUBSEQUENCES_TEST.java:51)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  10,test_6(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTS  11,test_7(java_testcases.junit.SUBSEQUENCES_TEST)
+%FAILED 11,test_7(java_testcases.junit.SUBSEQUENCES_TEST)
+%EXPECTS
+[[1,2,3,4],[1,2,3,5],[1,2,3,6],[1,2,3,7],[1,2,3,8],[1,2,3,9],[1,2,4,5],[1,2,4,6],[1,2,4,7],[1,2,4,8],[1,2,4,9],[1,2,5,6],[1,2,5,7],[1,2,5,8],[1,2,5,9],[1,2,6,7],[1,2,6,8],[1,2,6,9],[1,2,7,8],[1,2,7,9],[1,2,8,9],[1,3,4,5],[1,3,4,6],[1,3,4,7],[1,3,4,8],[1,3,4,9],[1,3,5,6],[1,3,5,7],[1,3,5,8],[1,3,5,9],[1,3,6,7],[1,3,6,8],[1,3,6,9],[1,3,7,8],[1,3,7,9],[1,3,8,9],[1,4,5,6],[1,4,5,7],[1,4,5,8],[1,4,5,9],[1,4,6,7],[1,4,6,8],[1,4,6,9],[1,4,7,8],[1,4,7,9],[1,4,8,9],[1,5,6,7],[1,5,6,8],[1,5,6,9],[1,5,7,8],[1,5,7,9],[1,5,8,9],[1,6,7,8],[1,6,7,9],[1,6,8,9],[1,7,8,9],[2,3,4,5],[2,3,4,6],[2,3,4,7],[2,3,4,8],[2,3,4,9],[2,3,5,6],[2,3,5,7],[2,3,5,8],[2,3,5,9],[2,3,6,7],[2,3,6,8],[2,3,6,9],[2,3,7,8],[2,3,7,9],[2,3,8,9],[2,4,5,6],[2,4,5,7],[2,4,5,8],[2,4,5,9],[2,4,6,7],[2,4,6,8],[2,4,6,9],[2,4,7,8],[2,4,7,9],[2,4,8,9],[2,5,6,7],[2,5,6,8],[2,5,6,9],[2,5,7,8],[2,5,7,9],[2,5,8,9],[2,6,7,8],[2,6,7,9],[2,6,8,9],[2,7,8,9],[3,4,5,6],[3,4,5,7],[3,4,5,8],[3,4,5,9],[3,4,6,7],[3,4,6,8],[3,4,6,9],[3,4,7,8],[3,4,7,9],[3,4,8,9],[3,5,6,7],[3,5,6,8],[3,5,6,9],[3,5,7,8],[3,5,7,9],[3,5,8,9],[3,6,7,8],[3,6,7,9],[3,6,8,9],[3,7,8,9],[4,5,6,7],[4,5,6,8],[4,5,6,9],[4,5,7,8],[4,5,7,9],[4,5,8,9],[4,6,7,8],[4,6,7,9],[4,6,8,9],[4,7,8,9],[5,6,7,8],[5,6,7,9],[5,6,8,9],[5,7,8,9],[6,7,8,9]]
+%EXPECTE
+%ACTUALS
+[]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[1,2,3,4],[1,2,3,5],[1,2,3,6],[1,2,3,7],[1,2,3,8],[1,2,3,9],[1,2,4,5],[1,2,4,6],[1,2,4,7],[1,2,4,8],[1,2,4,9],[1,2,5,6],[1,2,5,7],[1,2,5,8],[1,2,5,9],[1,2,6,7],[1,2,6,8],[1,2,6,9],[1,2,7,8],[1,2,7,9],[1,2,8,9],[1,3,4,5],[1,3,4,6],[1,3,4,7],[1,3,4,8],[1,3,4,9],[1,3,5,6],[1,3,5,7],[1,3,5,8],[1,3,5,9],[1,3,6,7],[1,3,6,8],[1,3,6,9],[1,3,7,8],[1,3,7,9],[1,3,8,9],[1,4,5,6],[1,4,5,7],[1,4,5,8],[1,4,5,9],[1,4,6,7],[1,4,6,8],[1,4,6,9],[1,4,7,8],[1,4,7,9],[1,4,8,9],[1,5,6,7],[1,5,6,8],[1,5,6,9],[1,5,7,8],[1,5,7,9],[1,5,8,9],[1,6,7,8],[1,6,7,9],[1,6,8,9],[1,7,8,9],[2,3,4,5],[2,3,4,6],[2,3,4,7],[2,3,4,8],[2,3,4,9],[2,3,5,6],[2,3,5,7],[2,3,5,8],[2,3,5,9],[2,3,6,7],[2,3,6,8],[2,3,6,9],[2,3,7,8],[2,3,7,9],[2,3,8,9],[2,4,5,6],[2,4,5,7],[2,4,5,8],[2,4,5,9],[2,4,6,7],[2,4,6,8],[2,4,6,9],[2,4,7,8],[2,4,7,9],[2,4,8,9],[2,5,6,7],[2,5,6,8],[2,5,6,9],[2,5,7,8],[2,5,7,9],[2,5,8,9],[2,6,7,8],[2,6,7,9],[2,6,8,9],[2,7,8,9],[3,4,5,6],[3,4,5,7],[3,4,5,8],[3,4,5,9],[3,4,6,7],[3,4,6,8],[3,4,6,9],[3,4,7,8],[3,4,7,9],[3,4,8,9],[3,5,6,7],[3,5,6,8],[3,5,6,9],[3,5,7,8],[3,5,7,9],[3,5,8,9],[3,6,7,8],[3,6,7,9],[3,6,8,9],[3,7,8,9],[4,5,6,7],[4,5,6,8],[4,5,6,9],[4,5,7,8],[4,5,7,9],[4,5,8,9],[4,6,7,8],[4,6,7,9],[4,6,8,9],[4,7,8,9],[5,6,7,8],[5,6,7,9],[5,6,8,9],[5,7,8,9],[6,7,8,9]]]&gt; but was:&lt;[[]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.SUBSEQUENCES_TEST.test_7(SUBSEQUENCES_TEST.java:58)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  11,test_7(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTS  12,test_8(java_testcases.junit.SUBSEQUENCES_TEST)
+%FAILED 12,test_8(java_testcases.junit.SUBSEQUENCES_TEST)
+%EXPECTS
+[[1],[2],[3],[4],[5],[6],[7],[8],[9]]
+%EXPECTE
+%ACTUALS
+[]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[1],[2],[3],[4],[5],[6],[7],[8],[9]]]&gt; but was:&lt;[[]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.SUBSEQUENCES_TEST.test_8(SUBSEQUENCES_TEST.java:65)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  12,test_8(java_testcases.junit.SUBSEQUENCES_TEST)
+%TESTS  13,test_9(java_testcases.junit.SUBSEQUENCES_TEST)
+%FAILED 13,test_9(java_testcases.junit.SUBSEQUENCES_TEST)
+%EXPECTS
+[[5,6,7,8,9,10,11],[5,6,7,8,9,10,12],[5,6,7,8,9,11,12],[5,6,7,8,10,11,12],[5,6,7,9,10,11,12],[5,6,8,9,10,11,12],[5,7,8,9,10,11,12],[6,7,8,9,10,11,12]]
+%EXPECTE
+%ACTUALS
+[]
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[[[5,6,7,8,9,10,11],[5,6,7,8,9,10,12],[5,6,7,8,9,11,12],[5,6,7,8,10,11,12],[5,6,7,9,10,11,12],[5,6,8,9,10,11,12],[5,7,8,9,10,11,12],[6,7,8,9,10,11,12]]]&gt; but was:&lt;[[]]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.SUBSEQUENCES_TEST.test_9(SUBSEQUENCES_TEST.java:72)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  13,test_9(java_testcases.junit.SUBSEQUENCES_TEST)
+%RUNTIME262
+</t>
+  </si>
+  <si>
+    <t>%TESTC  7 v2
+%TSTTREE1,java_testcases.junit.TO_BASE_TEST,true,7,false,-1,java_testcases.junit.TO_BASE_TEST,,
+%TSTTREE2,test_0(java_testcases.junit.TO_BASE_TEST),false,1,false,-1,test_0(java_testcases.junit.TO_BASE_TEST),,
+%TSTTREE3,test_1(java_testcases.junit.TO_BASE_TEST),false,1,false,-1,test_1(java_testcases.junit.TO_BASE_TEST),,
+%TSTTREE4,test_2(java_testcases.junit.TO_BASE_TEST),false,1,false,-1,test_2(java_testcases.junit.TO_BASE_TEST),,
+%TSTTREE5,test_3(java_testcases.junit.TO_BASE_TEST),false,1,false,-1,test_3(java_testcases.junit.TO_BASE_TEST),,
+%TSTTREE6,test_4(java_testcases.junit.TO_BASE_TEST),false,1,false,-1,test_4(java_testcases.junit.TO_BASE_TEST),,
+%TSTTREE7,test_5(java_testcases.junit.TO_BASE_TEST),false,1,false,-1,test_5(java_testcases.junit.TO_BASE_TEST),,
+%TSTTREE8,test_6(java_testcases.junit.TO_BASE_TEST),false,1,false,-1,test_6(java_testcases.junit.TO_BASE_TEST),,
+%TESTS  2,test_0(java_testcases.junit.TO_BASE_TEST)
+%FAILED 2,test_0(java_testcases.junit.TO_BASE_TEST)
+%EXPECTS
+1F
+%EXPECTE
+%ACTUALS
+F1
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[1F]&gt; but was:&lt;[F1]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.TO_BASE_TEST.test_0(TO_BASE_TEST.java:9)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  2,test_0(java_testcases.junit.TO_BASE_TEST)
+%TESTS  3,test_1(java_testcases.junit.TO_BASE_TEST)
+%FAILED 3,test_1(java_testcases.junit.TO_BASE_TEST)
+%EXPECTS
+101001
+%EXPECTE
+%ACTUALS
+100101
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;10[10]01&gt; but was:&lt;10[01]01&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.TO_BASE_TEST.test_1(TO_BASE_TEST.java:16)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  3,test_1(java_testcases.junit.TO_BASE_TEST)
+%TESTS  4,test_2(java_testcases.junit.TO_BASE_TEST)
+%FAILED 4,test_2(java_testcases.junit.TO_BASE_TEST)
+%EXPECTS
+134
+%EXPECTE
+%ACTUALS
+431
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[134]&gt; but was:&lt;[431]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.TO_BASE_TEST.test_2(TO_BASE_TEST.java:23)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  4,test_2(java_testcases.junit.TO_BASE_TEST)
+%TESTS  5,test_3(java_testcases.junit.TO_BASE_TEST)
+%FAILED 5,test_3(java_testcases.junit.TO_BASE_TEST)
+%EXPECTS
+14
+%EXPECTE
+%ACTUALS
+41
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[14]&gt; but was:&lt;[41]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.TO_BASE_TEST.test_3(TO_BASE_TEST.java:30)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  5,test_3(java_testcases.junit.TO_BASE_TEST)
+%TESTS  6,test_4(java_testcases.junit.TO_BASE_TEST)
+%FAILED 6,test_4(java_testcases.junit.TO_BASE_TEST)
+%EXPECTS
+2A
+%EXPECTE
+%ACTUALS
+A2
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[2A]&gt; but was:&lt;[A2]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.TO_BASE_TEST.test_4(TO_BASE_TEST.java:37)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  6,test_4(java_testcases.junit.TO_BASE_TEST)
+%TESTS  7,test_5(java_testcases.junit.TO_BASE_TEST)
+%FAILED 7,test_5(java_testcases.junit.TO_BASE_TEST)
+%EXPECTS
+E75
+%EXPECTE
+%ACTUALS
+57E
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[E75]&gt; but was:&lt;[57E]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.TO_BASE_TEST.test_5(TO_BASE_TEST.java:44)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  7,test_5(java_testcases.junit.TO_BASE_TEST)
+%TESTS  8,test_6(java_testcases.junit.TO_BASE_TEST)
+%FAILED 8,test_6(java_testcases.junit.TO_BASE_TEST)
+%EXPECTS
+749
+%EXPECTE
+%ACTUALS
+947
+%ACTUALE
+%TRACES 
+org.junit.ComparisonFailure: expected:&lt;[749]&gt; but was:&lt;[947]&gt;
+        at org.junit.Assert.assertEquals(Assert.java:117)
+        at org.junit.Assert.assertEquals(Assert.java:146)
+        at java_testcases.junit.TO_BASE_TEST.test_6(TO_BASE_TEST.java:51)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+        at java.base/jdk.internal.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+        at java.base/jdk.internal.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+        at java.base/java.lang.reflect.Method.invoke(Method.java:566)
+        at org.junit.runners.model.FrameworkMethod$1.runReflectiveCall(FrameworkMethod.java:59)
+        at org.junit.internal.runners.model.ReflectiveCallable.run(ReflectiveCallable.java:12)
+        at org.junit.runners.model.FrameworkMethod.invokeExplosively(FrameworkMethod.java:56)
+        at org.junit.internal.runners.statements.InvokeMethod.evaluate(InvokeMethod.java:17)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:299)
+        at org.junit.internal.runners.statements.FailOnTimeout$CallableStatement.call(FailOnTimeout.java:293)
+        at java.base/java.util.concurrent.FutureTask.run(FutureTask.java:264)
+        at java.base/java.lang.Thread.run(Thread.java:834)
+%TRACEE 
+%TESTE  8,test_6(java_testcases.junit.TO_BASE_TEST)
+%RUNTIME358</t>
   </si>
 </sst>
 </file>
@@ -5543,19 +8002,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="F43" zoomScale="59" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="51.5546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" customWidth="1"/>
+    <col min="8" max="8" width="51.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5590,7 +8049,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -5618,9 +8077,11 @@
       <c r="I2" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -5643,14 +8104,16 @@
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -5673,14 +8136,16 @@
         <v>21</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -5703,14 +8168,19 @@
         <v>26</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>301</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -5733,14 +8203,16 @@
         <v>31</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -5763,14 +8235,19 @@
         <v>36</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>302</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -5793,14 +8270,16 @@
         <v>41</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -5823,15 +8302,17 @@
         <v>46</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -5854,14 +8335,16 @@
         <v>51</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="J10" s="2"/>
+      <c r="J10" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -5884,15 +8367,19 @@
         <v>56</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
+      <c r="J11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>303</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>57</v>
       </c>
@@ -5915,14 +8402,19 @@
         <v>61</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>304</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -5945,14 +8437,16 @@
         <v>66</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="J13" s="2"/>
+      <c r="J13" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
@@ -5975,14 +8469,16 @@
         <v>71</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="J14" s="2"/>
+      <c r="J14" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -6005,14 +8501,16 @@
         <v>76</v>
       </c>
       <c r="H15" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="J15" s="2"/>
+      <c r="J15" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
@@ -6035,14 +8533,19 @@
         <v>81</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="J16" s="2"/>
+      <c r="J16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>305</v>
+      </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
@@ -6065,15 +8568,19 @@
         <v>86</v>
       </c>
       <c r="H17" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
+      <c r="J17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>306</v>
+      </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>87</v>
       </c>
@@ -6096,14 +8603,16 @@
         <v>91</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="J18" s="2"/>
+      <c r="J18" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>92</v>
       </c>
@@ -6126,15 +8635,17 @@
         <v>96</v>
       </c>
       <c r="H19" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="J19" s="5"/>
+      <c r="J19" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>97</v>
       </c>
@@ -6157,15 +8668,20 @@
         <v>101</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
+      <c r="J20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>102</v>
       </c>
@@ -6188,15 +8704,17 @@
         <v>106</v>
       </c>
       <c r="H21" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="J21" s="5"/>
+      <c r="J21" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>107</v>
       </c>
@@ -6219,14 +8737,20 @@
         <v>111</v>
       </c>
       <c r="H22" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="J22" s="2"/>
+      <c r="J22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>112</v>
       </c>
@@ -6249,15 +8773,20 @@
         <v>116</v>
       </c>
       <c r="H23" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="J23" s="5"/>
-      <c r="K23" s="6"/>
+      <c r="J23" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>117</v>
       </c>
@@ -6280,15 +8809,20 @@
         <v>121</v>
       </c>
       <c r="H24" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="J24" s="5"/>
-      <c r="K24" s="6"/>
+      <c r="J24" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>122</v>
       </c>
@@ -6308,15 +8842,17 @@
         <v>125</v>
       </c>
       <c r="H25" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="J25" s="5"/>
+      <c r="J25" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>126</v>
       </c>
@@ -6339,12 +8875,13 @@
         <v>130</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="2"/>
+      <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>131</v>
       </c>
@@ -6367,15 +8904,17 @@
         <v>135</v>
       </c>
       <c r="H27" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="J27" s="5"/>
+      <c r="J27" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>136</v>
       </c>
@@ -6398,15 +8937,17 @@
         <v>140</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="J28" s="5"/>
+      <c r="J28" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>141</v>
       </c>
@@ -6429,15 +8970,20 @@
         <v>145</v>
       </c>
       <c r="H29" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="I29" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="J29" s="5"/>
-      <c r="K29" s="6"/>
+      <c r="J29" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>146</v>
       </c>
@@ -6457,15 +9003,17 @@
         <v>149</v>
       </c>
       <c r="H30" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="J30" s="5"/>
+      <c r="J30" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>150</v>
       </c>
@@ -6488,14 +9036,17 @@
         <v>154</v>
       </c>
       <c r="H31" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I31" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="J31" s="2"/>
+      <c r="J31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>155</v>
       </c>
@@ -6518,15 +9069,17 @@
         <v>159</v>
       </c>
       <c r="H32" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="J32" s="5"/>
+      <c r="J32" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>160</v>
       </c>
@@ -6549,14 +9102,19 @@
         <v>164</v>
       </c>
       <c r="H33" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="J33" s="2"/>
+      <c r="J33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>312</v>
+      </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>165</v>
       </c>
@@ -6579,14 +9137,16 @@
         <v>169</v>
       </c>
       <c r="H34" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="J34" s="2"/>
+      <c r="J34" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>170</v>
       </c>
@@ -6609,14 +9169,19 @@
         <v>174</v>
       </c>
       <c r="H35" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="J35" s="2"/>
+      <c r="J35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>313</v>
+      </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>175</v>
       </c>
@@ -6639,15 +9204,19 @@
         <v>179</v>
       </c>
       <c r="H36" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J36" s="5"/>
-      <c r="K36" s="6"/>
+      <c r="J36" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>314</v>
+      </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>180</v>
       </c>
@@ -6670,14 +9239,19 @@
         <v>184</v>
       </c>
       <c r="H37" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="J37" s="2"/>
+      <c r="J37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>315</v>
+      </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>185</v>
       </c>
@@ -6700,14 +9274,16 @@
         <v>189</v>
       </c>
       <c r="H38" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="J38" s="2"/>
+      <c r="J38" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>190</v>
       </c>
@@ -6730,15 +9306,19 @@
         <v>194</v>
       </c>
       <c r="H39" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="J39" s="5"/>
-      <c r="K39" s="6"/>
+      <c r="J39" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>316</v>
+      </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>195</v>
       </c>
@@ -6761,14 +9341,16 @@
         <v>199</v>
       </c>
       <c r="H40" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="I40" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="J40" s="2"/>
+      <c r="J40" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>200</v>
       </c>
@@ -6791,14 +9373,19 @@
         <v>204</v>
       </c>
       <c r="H41" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="I41" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="J41" s="2"/>
+      <c r="J41" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>205</v>
       </c>
@@ -6821,12 +9408,12 @@
         <v>209</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>210</v>
       </c>
@@ -6849,12 +9436,14 @@
         <v>214</v>
       </c>
       <c r="H43" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="I43" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="J43" s="2"/>
+      <c r="J43" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H44" s="2"/>
@@ -6863,7 +9452,7 @@
       </c>
       <c r="J44" s="2">
         <f>COUNTIF(J2:J43,TRUE)</f>
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6873,17 +9462,17 @@
       </c>
       <c r="J45" s="2">
         <f>COUNTIF(J2:J43,FALSE)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H46" s="2"/>
       <c r="I46" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="J46" s="2" t="e">
+        <v>299</v>
+      </c>
+      <c r="J46" s="2">
         <f>J44/(J44+J45)*100</f>
-        <v>#DIV/0!</v>
+        <v>57.499999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>